<commit_message>
updated to link to properly named pages
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@8781 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="11835"/>
+    <workbookView xWindow="2325" yWindow="4530" windowWidth="24915" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="113">
   <si>
     <t>careteam-daf-core</t>
   </si>
@@ -39,9 +39,6 @@
     <t>practitioner-daf-core</t>
   </si>
   <si>
-    <t>profile page root</t>
-  </si>
-  <si>
     <t>profile definition page</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>AllergyIntolerance</t>
   </si>
   <si>
-    <t>base resource</t>
-  </si>
-  <si>
     <t>allergyintolerance-daf-core</t>
   </si>
   <si>
@@ -327,9 +321,6 @@
     <t>Observation</t>
   </si>
   <si>
-    <t>core profile title</t>
-  </si>
-  <si>
     <t>Conformance</t>
   </si>
   <si>
@@ -352,6 +343,18 @@
   </si>
   <si>
     <t>MHD</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Core Profile Title</t>
+  </si>
+  <si>
+    <t>Base Resource</t>
+  </si>
+  <si>
+    <t>Profile Page</t>
   </si>
 </sst>
 </file>
@@ -693,37 +696,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="61.5703125" customWidth="1"/>
+    <col min="4" max="4" width="61.5703125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -731,19 +737,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -751,19 +757,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -771,19 +777,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -791,56 +797,59 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -848,364 +857,359 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
         <v>107</v>
-      </c>
-      <c r="D9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26">
-        <v>24</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create a new profile page template with text summary.
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@8783 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="4530" windowWidth="24915" windowHeight="11835"/>
+    <workbookView xWindow="-15" yWindow="-330" windowWidth="24915" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="133">
   <si>
     <t>careteam-daf-core</t>
   </si>
@@ -120,12 +120,6 @@
     <t>procedure-daf-core-profile-spreadsheet.xml</t>
   </si>
   <si>
-    <t>Allergies</t>
-  </si>
-  <si>
-    <t>Assess and Plan</t>
-  </si>
-  <si>
     <t>CareTeam</t>
   </si>
   <si>
@@ -240,21 +234,12 @@
     <t>daf-core-procedure</t>
   </si>
   <si>
-    <t>Problems and Concerns</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
-    <t>UDI</t>
-  </si>
-  <si>
     <t>Device</t>
   </si>
   <si>
-    <t>Lab Reports</t>
-  </si>
-  <si>
     <t>DiagnosticReport</t>
   </si>
   <si>
@@ -342,19 +327,94 @@
     <t>daf-core-documentreference</t>
   </si>
   <si>
-    <t>MHD</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Core Profile Title</t>
-  </si>
-  <si>
     <t>Base Resource</t>
   </si>
   <si>
     <t>Profile Page</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>core-allergyintolerance</t>
+  </si>
+  <si>
+    <t>core-careplan</t>
+  </si>
+  <si>
+    <t>core-careteam</t>
+  </si>
+  <si>
+    <t>core-condition</t>
+  </si>
+  <si>
+    <t>core-conformance</t>
+  </si>
+  <si>
+    <t>core-device</t>
+  </si>
+  <si>
+    <t>core-diagnosticreport</t>
+  </si>
+  <si>
+    <t>core-documentreference</t>
+  </si>
+  <si>
+    <t>core-goals</t>
+  </si>
+  <si>
+    <t>core-immunization</t>
+  </si>
+  <si>
+    <t>core-location</t>
+  </si>
+  <si>
+    <t>core-medication</t>
+  </si>
+  <si>
+    <t>core-medicationadministration</t>
+  </si>
+  <si>
+    <t>core-medicationdispense</t>
+  </si>
+  <si>
+    <t>core-medicationorder</t>
+  </si>
+  <si>
+    <t>core-medicationstatement</t>
+  </si>
+  <si>
+    <t>core-observation-results</t>
+  </si>
+  <si>
+    <t>core-observation-resultsv2</t>
+  </si>
+  <si>
+    <t>core-observation-smokingstatus</t>
+  </si>
+  <si>
+    <t>core-observation-vitalsigns</t>
+  </si>
+  <si>
+    <t>core-organization</t>
+  </si>
+  <si>
+    <t>core-patient</t>
+  </si>
+  <si>
+    <t>core-practitioner</t>
+  </si>
+  <si>
+    <t>core-procedure</t>
+  </si>
+  <si>
+    <t>DiagnosticReport-Results</t>
+  </si>
+  <si>
+    <t>Core Profile Title = id</t>
   </si>
 </sst>
 </file>
@@ -696,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,32 +772,35 @@
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -751,8 +814,11 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -760,27 +826,30 @@
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -789,118 +858,136 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>52</v>
+      </c>
+      <c r="G4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>98</v>
+      </c>
+      <c r="G6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>55</v>
+      </c>
+      <c r="G8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -909,38 +996,44 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -949,198 +1042,228 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>61</v>
+      </c>
+      <c r="G15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="G16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
         <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>66</v>
+      </c>
+      <c r="G20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
         <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>67</v>
+      </c>
+      <c r="G21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
         <v>30</v>
@@ -1149,18 +1272,21 @@
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>68</v>
+      </c>
+      <c r="G22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
@@ -1169,18 +1295,21 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -1189,27 +1318,33 @@
         <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DAF Core creation - device, goal, careteam
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@8884 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FHIR_Build\guides\daf2\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-330" windowWidth="24915" windowHeight="11835"/>
   </bookViews>
@@ -12,12 +17,12 @@
     <sheet name="Extensions" sheetId="3" r:id="rId3"/>
     <sheet name="ValueSets" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="196">
   <si>
     <t>careteam-daf-core</t>
   </si>
@@ -445,9 +450,6 @@
     <t>Conformance(Conformance)</t>
   </si>
   <si>
-    <t>Both…</t>
-  </si>
-  <si>
     <t>DocumentReference (DocumentReference)</t>
   </si>
   <si>
@@ -599,13 +601,22 @@
   </si>
   <si>
     <t>medicationadministration</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Created, not hooked in</t>
+  </si>
+  <si>
+    <t>created</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +705,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -740,7 +759,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -772,9 +791,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -806,6 +843,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -981,19 +1036,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" customWidth="1"/>
@@ -1006,7 +1061,7 @@
     <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -1026,13 +1081,13 @@
         <v>135</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>73</v>
@@ -1050,7 +1105,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1060,11 +1115,14 @@
       <c r="C2" t="s">
         <v>137</v>
       </c>
+      <c r="D2" t="s">
+        <v>193</v>
+      </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>8</v>
@@ -1083,7 +1141,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1093,14 +1151,17 @@
       <c r="C3" t="s">
         <v>139</v>
       </c>
+      <c r="D3" t="s">
+        <v>193</v>
+      </c>
       <c r="G3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J3" t="s">
         <v>12</v>
@@ -1119,7 +1180,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1129,14 +1190,17 @@
       <c r="C4" t="s">
         <v>139</v>
       </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -1155,7 +1219,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1163,16 +1227,16 @@
         <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H5" t="s">
         <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J5" t="s">
         <v>67</v>
@@ -1191,24 +1255,24 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75">
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
         <v>143</v>
       </c>
-      <c r="C6" t="s">
-        <v>144</v>
-      </c>
       <c r="G6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H6" t="s">
         <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J6" t="s">
         <v>69</v>
@@ -1227,60 +1291,63 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75">
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>?-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
         <v>137</v>
       </c>
+      <c r="D8" t="s">
+        <v>195</v>
+      </c>
       <c r="G8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H8" t="s">
         <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J8" t="s">
         <v>50</v>
@@ -1299,21 +1366,24 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75">
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
         <v>137</v>
       </c>
+      <c r="D9" t="s">
+        <v>195</v>
+      </c>
       <c r="H9" t="s">
         <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J9" t="s">
         <v>51</v>
@@ -1332,21 +1402,24 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75">
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" t="s">
         <v>137</v>
       </c>
+      <c r="D10" t="s">
+        <v>195</v>
+      </c>
       <c r="G10" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10" t="s">
         <v>164</v>
-      </c>
-      <c r="H10" t="s">
-        <v>165</v>
       </c>
       <c r="J10" t="s">
         <v>48</v>
@@ -1356,42 +1429,45 @@
         <v>-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L10" t="s">
+        <v>165</v>
+      </c>
+      <c r="M10" t="s">
         <v>166</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>167</v>
       </c>
-      <c r="N10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75">
+    </row>
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
         <v>137</v>
       </c>
+      <c r="D11" t="s">
+        <v>195</v>
+      </c>
       <c r="H11" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1401,11 +1477,14 @@
       <c r="C12" t="s">
         <v>137</v>
       </c>
+      <c r="D12" t="s">
+        <v>195</v>
+      </c>
       <c r="H12" t="s">
         <v>97</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J12" t="s">
         <v>49</v>
@@ -1424,7 +1503,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75">
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1434,11 +1513,14 @@
       <c r="C13" t="s">
         <v>137</v>
       </c>
+      <c r="D13" t="s">
+        <v>195</v>
+      </c>
       <c r="H13" t="s">
         <v>54</v>
       </c>
       <c r="I13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J13" t="s">
         <v>66</v>
@@ -1457,21 +1539,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75">
+    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="D14" t="s">
+        <v>195</v>
       </c>
       <c r="H14" t="s">
         <v>52</v>
       </c>
       <c r="I14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J14" t="s">
         <v>52</v>
@@ -1490,33 +1575,36 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75">
+    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
         <v>139</v>
       </c>
+      <c r="D15" t="s">
+        <v>195</v>
+      </c>
       <c r="H15" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1526,11 +1614,14 @@
       <c r="C16" t="s">
         <v>139</v>
       </c>
+      <c r="D16" t="s">
+        <v>195</v>
+      </c>
       <c r="H16" t="s">
         <v>64</v>
       </c>
       <c r="I16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J16" t="s">
         <v>64</v>
@@ -1549,7 +1640,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75">
+    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1559,11 +1650,14 @@
       <c r="C17" t="s">
         <v>139</v>
       </c>
+      <c r="D17" t="s">
+        <v>195</v>
+      </c>
       <c r="H17" t="s">
         <v>65</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J17" t="s">
         <v>65</v>
@@ -1582,7 +1676,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75">
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1592,11 +1686,14 @@
       <c r="C18" t="s">
         <v>139</v>
       </c>
+      <c r="D18" t="s">
+        <v>195</v>
+      </c>
       <c r="H18" t="s">
         <v>53</v>
       </c>
       <c r="I18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J18" t="s">
         <v>53</v>
@@ -1615,21 +1712,24 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75">
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="D19" t="s">
+        <v>195</v>
       </c>
       <c r="H19" t="s">
         <v>58</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J19" t="s">
         <v>58</v>
@@ -1648,21 +1748,24 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75">
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
         <v>137</v>
       </c>
+      <c r="D20" t="s">
+        <v>193</v>
+      </c>
       <c r="H20" t="s">
         <v>59</v>
       </c>
       <c r="I20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J20" t="s">
         <v>59</v>
@@ -1681,21 +1784,24 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75">
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C21" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="D21" t="s">
+        <v>195</v>
       </c>
       <c r="H21" t="s">
         <v>60</v>
       </c>
       <c r="I21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J21" t="s">
         <v>60</v>
@@ -1714,21 +1820,24 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75">
+    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" t="s">
         <v>139</v>
       </c>
+      <c r="D22" t="s">
+        <v>195</v>
+      </c>
       <c r="H22" t="s">
         <v>47</v>
       </c>
       <c r="I22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J22" t="s">
         <v>47</v>
@@ -1747,21 +1856,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75">
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
         <v>139</v>
       </c>
+      <c r="D23" t="s">
+        <v>195</v>
+      </c>
       <c r="H23" t="s">
         <v>61</v>
       </c>
       <c r="I23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J23" t="s">
         <v>61</v>
@@ -1780,21 +1892,24 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75">
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
         <v>139</v>
       </c>
+      <c r="D24" t="s">
+        <v>195</v>
+      </c>
       <c r="H24" t="s">
         <v>56</v>
       </c>
       <c r="I24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J24" t="s">
         <v>66</v>
@@ -1813,21 +1928,24 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75">
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" t="s">
         <v>137</v>
       </c>
+      <c r="D25" t="s">
+        <v>195</v>
+      </c>
       <c r="H25" t="s">
         <v>57</v>
       </c>
       <c r="I25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J25" t="s">
         <v>66</v>
@@ -1846,15 +1964,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75">
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H28" t="s">
         <v>63</v>
       </c>
       <c r="I28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J28" t="s">
         <v>63</v>
@@ -1873,15 +1991,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75">
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H29" t="s">
         <v>62</v>
       </c>
       <c r="I29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J29" t="s">
         <v>62</v>
@@ -1900,9 +2018,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H30" t="s">
         <v>55</v>
@@ -1934,14 +2052,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
@@ -1949,7 +2067,7 @@
     <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -1960,7 +2078,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -1971,7 +2089,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -1995,7 +2113,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -2019,7 +2137,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -2043,7 +2161,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -2067,7 +2185,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2091,12 +2209,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2109,13 +2227,13 @@
         <v>125</v>
       </c>
       <c r="F8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2139,7 +2257,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -2163,7 +2281,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -2187,7 +2305,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -2211,7 +2329,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -2235,7 +2353,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -2259,7 +2377,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -2283,7 +2401,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -2307,7 +2425,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -2331,7 +2449,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -2355,7 +2473,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -2379,7 +2497,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -2403,7 +2521,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -2427,7 +2545,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>115</v>
       </c>
@@ -2451,7 +2569,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -2475,7 +2593,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -2499,7 +2617,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -2523,7 +2641,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -2547,13 +2665,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="9"/>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="9"/>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
     </row>
   </sheetData>
@@ -2565,26 +2683,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update dad core profiles spreadsheet - add value set tracker,  added core value sets for allergies
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@8893 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FHIR_Build\guides\daf2\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-330" windowWidth="24915" windowHeight="11835"/>
+    <workbookView xWindow="-15" yWindow="-330" windowWidth="24915" windowHeight="11835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="Extensions" sheetId="3" r:id="rId3"/>
     <sheet name="ValueSets" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027" calcOnSave="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="209">
   <si>
     <t>careteam-daf-core</t>
   </si>
@@ -610,13 +605,52 @@
   </si>
   <si>
     <t>created</t>
+  </si>
+  <si>
+    <t>Valueset id</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>XPDY0002: Cannot evaluate function 'fn:root', because the context node is undefined</t>
+  </si>
+  <si>
+    <t>daf-core-substance-ndfrt</t>
+  </si>
+  <si>
+    <t>daf-core-substance-rxnorm</t>
+  </si>
+  <si>
+    <t>daf-core-substance-sct</t>
+  </si>
+  <si>
+    <t>daf-core-substance-unii</t>
+  </si>
+  <si>
+    <t>daf-core-substance</t>
+  </si>
+  <si>
+    <t>DAF Core Substance ND-FRT codes</t>
+  </si>
+  <si>
+    <t>DAF Core Substance RxNorm Codes</t>
+  </si>
+  <si>
+    <t>DAF Core SNOMED CT Substances Other Than Clinical Drugs</t>
+  </si>
+  <si>
+    <t>DAF Core Substance UNII Codes</t>
+  </si>
+  <si>
+    <t>DAF Core Substance-Reactant for Intolerance and Negation Codes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -699,6 +733,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,7 +794,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -791,27 +826,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -843,24 +860,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1036,14 +1035,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
@@ -1061,7 +1060,7 @@
     <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1180,7 +1179,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1219,7 +1218,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.75">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.75">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.75">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1402,7 +1401,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.75">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1438,7 +1437,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.75">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15.75">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1575,7 +1574,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1640,7 +1639,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1676,7 +1675,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1712,7 +1711,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1784,7 +1783,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1820,7 +1819,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1856,7 +1855,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -1928,7 +1927,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -1964,7 +1963,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75">
       <c r="B28" s="6" t="s">
         <v>161</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75">
       <c r="B29" s="6" t="s">
         <v>161</v>
       </c>
@@ -2018,7 +2017,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="B30" t="s">
         <v>160</v>
       </c>
@@ -2052,14 +2051,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
@@ -2067,7 +2066,7 @@
     <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2078,7 +2077,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -2161,7 +2160,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -2185,7 +2184,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2209,7 +2208,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>168</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2257,7 +2256,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -2281,7 +2280,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -2305,7 +2304,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -2329,7 +2328,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -2353,7 +2352,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -2401,7 +2400,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -2425,7 +2424,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -2449,7 +2448,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -2497,7 +2496,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -2521,7 +2520,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -2545,7 +2544,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>115</v>
       </c>
@@ -2569,7 +2568,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -2593,7 +2592,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -2617,7 +2616,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -2641,7 +2640,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -2665,13 +2664,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="B32" s="9"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2">
       <c r="B33" s="9"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2">
       <c r="B35" s="1"/>
     </row>
   </sheetData>
@@ -2683,27 +2682,321 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="99.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="8">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8">
+        <v>10</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="8">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="8">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="8">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="8">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="8">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="8">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="8">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="8">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="8">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="8">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added core value sets for allergies, updated url in value sets
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@8905 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="215">
   <si>
     <t>careteam-daf-core</t>
   </si>
@@ -644,6 +644,24 @@
   </si>
   <si>
     <t>DAF Core Substance-Reactant for Intolerance and Negation Codes</t>
+  </si>
+  <si>
+    <t>substance-ndfrt</t>
+  </si>
+  <si>
+    <t>substance-rxnorm</t>
+  </si>
+  <si>
+    <t>substance-sct</t>
+  </si>
+  <si>
+    <t>substance-unii</t>
+  </si>
+  <si>
+    <t>substance</t>
+  </si>
+  <si>
+    <t>id root</t>
   </si>
 </sst>
 </file>
@@ -2695,22 +2713,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="99.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="3" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="99.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -2721,10 +2739,13 @@
         <v>196</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2735,10 +2756,13 @@
         <v>199</v>
       </c>
       <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2749,10 +2773,13 @@
         <v>200</v>
       </c>
       <c r="D3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -2763,10 +2790,13 @@
         <v>201</v>
       </c>
       <c r="D4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2777,10 +2807,13 @@
         <v>202</v>
       </c>
       <c r="D5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="8">
         <v>1</v>
       </c>
@@ -2791,10 +2824,13 @@
         <v>203</v>
       </c>
       <c r="D6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E6" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -2802,7 +2838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -2810,7 +2846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -2818,7 +2854,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="8">
         <v>5</v>
       </c>
@@ -2826,7 +2862,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="8">
         <v>6</v>
       </c>
@@ -2834,7 +2870,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="8">
         <v>7</v>
       </c>
@@ -2842,7 +2878,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="8">
         <v>8</v>
       </c>
@@ -2850,7 +2886,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="8">
         <v>9</v>
       </c>
@@ -2858,7 +2894,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="8">
         <v>10</v>
       </c>
@@ -2866,7 +2902,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="8">
         <v>11</v>
       </c>
@@ -2874,7 +2910,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="8">
         <v>12</v>
       </c>
@@ -2882,18 +2918,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="8">
         <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" s="8">
         <v>14</v>
       </c>
@@ -2901,7 +2937,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" s="8">
         <v>15</v>
       </c>
@@ -2909,7 +2945,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="8">
         <v>16</v>
       </c>
@@ -2917,7 +2953,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="8">
         <v>17</v>
       </c>
@@ -2925,7 +2961,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -2933,7 +2969,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" s="8">
         <v>19</v>
       </c>
@@ -2941,7 +2977,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" s="8">
         <v>20</v>
       </c>
@@ -2949,7 +2985,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" s="8">
         <v>21</v>
       </c>
@@ -2957,7 +2993,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="8">
         <v>22</v>
       </c>
@@ -2965,7 +3001,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="8">
         <v>23</v>
       </c>
@@ -2973,7 +3009,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="8">
         <v>24</v>
       </c>
@@ -2981,7 +3017,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="B32" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
update profiles spreadsheet.  created md templates
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@8951 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26606"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/build/guides/daf2/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-330" windowWidth="24915" windowHeight="11835" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24920" windowHeight="11840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
-    <sheet name="Profiles-links" sheetId="2" r:id="rId2"/>
-    <sheet name="Extensions" sheetId="3" r:id="rId3"/>
-    <sheet name="ValueSets" sheetId="4" r:id="rId4"/>
+    <sheet name="exampletypesformappng" sheetId="5" r:id="rId2"/>
+    <sheet name="Profiles-links" sheetId="2" r:id="rId3"/>
+    <sheet name="Extensions" sheetId="3" r:id="rId4"/>
+    <sheet name="ValueSets" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="228">
   <si>
     <t>careteam-daf-core</t>
   </si>
@@ -463,15 +474,9 @@
     <t>Implantable Devices/UDI (Device)</t>
   </si>
   <si>
-    <t>Laboratory Results</t>
-  </si>
-  <si>
     <t>Location (Location)</t>
   </si>
   <si>
-    <t>Medications</t>
-  </si>
-  <si>
     <t>Organization (Organization)</t>
   </si>
   <si>
@@ -662,13 +667,58 @@
   </si>
   <si>
     <t>id root</t>
+  </si>
+  <si>
+    <t>build out with examples and valueset to model</t>
+  </si>
+  <si>
+    <t>core-endpoint</t>
+  </si>
+  <si>
+    <t>Laboratory Results-DiagnosticReport</t>
+  </si>
+  <si>
+    <t>Laboratory Results-Observation</t>
+  </si>
+  <si>
+    <t>Example id</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>.html</t>
+  </si>
+  <si>
+    <t>-xml.html</t>
+  </si>
+  <si>
+    <t>-json.html</t>
+  </si>
+  <si>
+    <t>file-extension</t>
+  </si>
+  <si>
+    <t>include text</t>
+  </si>
+  <si>
+    <t>{% core-example-template.html %}</t>
+  </si>
+  <si>
+    <t>{% core-example-json-template.html %}</t>
+  </si>
+  <si>
+    <t>{% core-example-xml-template.html %}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,7 +769,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -727,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -743,15 +793,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,12 +863,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -844,14 +895,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -878,6 +930,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1053,32 +1106,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" customWidth="1"/>
-    <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" customWidth="1"/>
+    <col min="8" max="8" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.5" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="57" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -1097,14 +1151,14 @@
       <c r="F1" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>162</v>
+      <c r="G1" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>73</v>
@@ -1121,25 +1175,31 @@
       <c r="N1" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75">
-      <c r="A2" s="8">
+      <c r="O1" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="12" t="s">
         <v>136</v>
       </c>
       <c r="C2" t="s">
         <v>137</v>
       </c>
-      <c r="D2" t="s">
-        <v>193</v>
+      <c r="D2" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>213</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>8</v>
@@ -1157,34 +1217,37 @@
       <c r="N2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75">
-      <c r="A3" s="8">
+      <c r="O2" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="12" t="s">
         <v>138</v>
       </c>
       <c r="C3" t="s">
         <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J3" t="s">
         <v>12</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K30" si="0">I3&amp;"-daf-core-profile-spreadsheet.xml"</f>
+        <f t="shared" ref="K3:K28" si="0">I3&amp;"-daf-core-profile-spreadsheet.xml"</f>
         <v>careplan-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L3" t="s">
@@ -1196,28 +1259,31 @@
       <c r="N3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75">
-      <c r="A4" s="8">
+      <c r="O3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="12" t="s">
         <v>140</v>
       </c>
       <c r="C4" t="s">
         <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -1235,25 +1301,28 @@
       <c r="N4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="8">
+      <c r="O4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="12" t="s">
         <v>141</v>
       </c>
       <c r="C5" t="s">
         <v>143</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H5" t="s">
         <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J5" t="s">
         <v>67</v>
@@ -1271,25 +1340,28 @@
       <c r="N5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="8">
+      <c r="O5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="12" t="s">
         <v>142</v>
       </c>
       <c r="C6" t="s">
         <v>143</v>
       </c>
       <c r="G6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H6" t="s">
         <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J6" t="s">
         <v>69</v>
@@ -1307,64 +1379,67 @@
       <c r="N6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="8">
+      <c r="O6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="12" t="s">
         <v>144</v>
       </c>
       <c r="C7" t="s">
         <v>143</v>
       </c>
       <c r="H7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>?-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N7" t="s">
-        <v>159</v>
+        <v>214</v>
       </c>
       <c r="O7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="8">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="12" t="s">
         <v>145</v>
       </c>
       <c r="C8" t="s">
         <v>137</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H8" t="s">
         <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J8" t="s">
         <v>50</v>
@@ -1382,25 +1457,28 @@
       <c r="N8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="8">
+      <c r="O8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="12" t="s">
         <v>146</v>
       </c>
       <c r="C9" t="s">
         <v>137</v>
       </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H9" t="s">
         <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J9" t="s">
         <v>51</v>
@@ -1418,25 +1496,28 @@
       <c r="N9" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="8">
+      <c r="O9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="12" t="s">
         <v>147</v>
       </c>
       <c r="C10" t="s">
         <v>137</v>
       </c>
       <c r="D10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J10" t="s">
         <v>48</v>
@@ -1446,616 +1527,600 @@
         <v>-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L10" t="s">
+        <v>163</v>
+      </c>
+      <c r="M10" t="s">
+        <v>164</v>
+      </c>
+      <c r="N10" t="s">
         <v>165</v>
       </c>
-      <c r="M10" t="s">
-        <v>166</v>
-      </c>
-      <c r="N10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="8">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>148</v>
+      <c r="O10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>11</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>215</v>
       </c>
       <c r="C11" t="s">
         <v>137</v>
       </c>
       <c r="D11" t="s">
-        <v>195</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75">
-      <c r="A12" s="8">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="H11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J11" t="s">
         <v>49</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>diagnosticreport-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" t="s">
+        <v>79</v>
+      </c>
+      <c r="O11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>12</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>216</v>
       </c>
       <c r="C12" t="s">
         <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H12" t="s">
-        <v>97</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>171</v>
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>180</v>
       </c>
       <c r="J12" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>diagnosticreport-daf-core-profile-spreadsheet.xml</v>
+        <v>resultobs-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>13</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" t="s">
+        <v>181</v>
+      </c>
+      <c r="J13" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>location-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" t="s">
+        <v>83</v>
+      </c>
+      <c r="O13" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
         <v>15</v>
       </c>
-      <c r="M12" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75">
-      <c r="A13" s="8">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" t="s">
-        <v>195</v>
-      </c>
-      <c r="H13" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" t="s">
-        <v>182</v>
-      </c>
-      <c r="J13" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="0"/>
-        <v>resultobs-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="15.75">
-      <c r="A14" s="8">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>149</v>
+      <c r="B14" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H14" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="I14" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v>location-daf-core-profile-spreadsheet.xml</v>
+        <v>medicationorder-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L14" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="M14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.75">
-      <c r="A15" s="8">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>150</v>
+        <v>87</v>
+      </c>
+      <c r="O14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>16</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>139</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75">
-      <c r="A16" s="8">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>64</v>
+        <v>193</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="J15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>medicationstatement-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L15" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" t="s">
+        <v>88</v>
+      </c>
+      <c r="O15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>17</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>139</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="I16" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="J16" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
-        <v>medicationorder-daf-core-profile-spreadsheet.xml</v>
+        <v>medication-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" t="s">
+        <v>84</v>
+      </c>
+      <c r="O16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>18</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" t="s">
+        <v>193</v>
+      </c>
+      <c r="H17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>organization-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" t="s">
+        <v>93</v>
+      </c>
+      <c r="O17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>19</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" t="s">
+        <v>191</v>
+      </c>
+      <c r="H18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" t="s">
+        <v>173</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>patient-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M18" t="s">
+        <v>44</v>
+      </c>
+      <c r="N18" t="s">
+        <v>94</v>
+      </c>
+      <c r="O18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
         <v>20</v>
       </c>
-      <c r="M16" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15.75">
-      <c r="A17" s="8">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D17" t="s">
-        <v>195</v>
-      </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="J17" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="0"/>
-        <v>medicationstatement-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L17" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" t="s">
-        <v>38</v>
-      </c>
-      <c r="N17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15.75">
-      <c r="A18" s="8">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D18" t="s">
-        <v>195</v>
-      </c>
-      <c r="H18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" t="s">
-        <v>179</v>
-      </c>
-      <c r="J18" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="0"/>
-        <v>medication-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L18" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15.75">
-      <c r="A19" s="8">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="12" t="s">
         <v>151</v>
       </c>
       <c r="C19" t="s">
         <v>143</v>
       </c>
       <c r="D19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H19" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>184</v>
+        <v>60</v>
+      </c>
+      <c r="I19" t="s">
+        <v>183</v>
       </c>
       <c r="J19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
-        <v>organization-daf-core-profile-spreadsheet.xml</v>
+        <v>pract-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L19" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="8">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="O19" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>21</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>152</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D20" t="s">
         <v>193</v>
       </c>
       <c r="H20" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="I20" t="s">
+        <v>171</v>
+      </c>
+      <c r="J20" t="s">
+        <v>47</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>condition-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" t="s">
+        <v>77</v>
+      </c>
+      <c r="O20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>22</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" t="s">
         <v>175</v>
       </c>
-      <c r="J20" t="s">
-        <v>59</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="0"/>
-        <v>patient-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L20" t="s">
-        <v>5</v>
-      </c>
-      <c r="M20" t="s">
-        <v>44</v>
-      </c>
-      <c r="N20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15.75">
-      <c r="A21" s="8">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" t="s">
-        <v>195</v>
-      </c>
-      <c r="H21" t="s">
-        <v>60</v>
-      </c>
-      <c r="I21" t="s">
-        <v>185</v>
-      </c>
       <c r="J21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
-        <v>pract-daf-core-profile-spreadsheet.xml</v>
+        <v>procedure-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L21" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="M21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="15.75">
-      <c r="A22" s="8">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="O21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>23</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>154</v>
       </c>
       <c r="C22" t="s">
         <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H22" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="I22" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="J22" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="0"/>
-        <v>condition-daf-core-profile-spreadsheet.xml</v>
+        <v>smokingstatus-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L22" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="M22" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="15.75">
-      <c r="A23" s="8">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="O22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>24</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>155</v>
       </c>
       <c r="C23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J23" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
-        <v>procedure-daf-core-profile-spreadsheet.xml</v>
+        <v>vitalsigns-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15.75">
-      <c r="A24" s="8">
+        <v>92</v>
+      </c>
+      <c r="O23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H26" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" t="s">
+        <v>189</v>
+      </c>
+      <c r="J26" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>medicationdispense-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L26" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" t="s">
+        <v>190</v>
+      </c>
+      <c r="J27" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>medicationadministration-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M27" t="s">
+        <v>35</v>
+      </c>
+      <c r="N27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L28" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C24" t="s">
-        <v>139</v>
-      </c>
-      <c r="D24" t="s">
-        <v>195</v>
-      </c>
-      <c r="H24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" t="s">
-        <v>181</v>
-      </c>
-      <c r="J24" t="s">
-        <v>66</v>
-      </c>
-      <c r="K24" t="str">
-        <f t="shared" si="0"/>
-        <v>smokingstatus-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L24" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" t="s">
-        <v>41</v>
-      </c>
-      <c r="N24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75">
-      <c r="A25" s="8">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" t="s">
-        <v>195</v>
-      </c>
-      <c r="H25" t="s">
-        <v>57</v>
-      </c>
-      <c r="I25" t="s">
-        <v>178</v>
-      </c>
-      <c r="J25" t="s">
-        <v>66</v>
-      </c>
-      <c r="K25" t="str">
-        <f t="shared" si="0"/>
-        <v>vitalsigns-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L25" t="s">
-        <v>25</v>
-      </c>
-      <c r="M25" t="s">
-        <v>42</v>
-      </c>
-      <c r="N25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="15.75">
-      <c r="B28" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H28" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28" t="s">
-        <v>191</v>
-      </c>
-      <c r="J28" t="s">
-        <v>63</v>
-      </c>
-      <c r="K28" t="str">
-        <f t="shared" si="0"/>
-        <v>medicationdispense-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L28" t="s">
-        <v>19</v>
-      </c>
       <c r="M28" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="N28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="15.75">
-      <c r="B29" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H29" t="s">
-        <v>62</v>
-      </c>
-      <c r="I29" t="s">
-        <v>192</v>
-      </c>
-      <c r="J29" t="s">
-        <v>62</v>
-      </c>
-      <c r="K29" t="str">
-        <f t="shared" si="0"/>
-        <v>medicationadministration-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L29" t="s">
-        <v>18</v>
-      </c>
-      <c r="M29" t="s">
-        <v>35</v>
-      </c>
-      <c r="N29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="B30" t="s">
-        <v>160</v>
-      </c>
-      <c r="H30" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" t="s">
-        <v>66</v>
-      </c>
-      <c r="K30" t="str">
-        <f t="shared" si="0"/>
-        <v>-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L30" t="s">
-        <v>23</v>
-      </c>
-      <c r="M30" t="s">
-        <v>40</v>
-      </c>
-      <c r="N30" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2069,22 +2134,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2095,7 +2211,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -2106,7 +2222,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2130,7 +2246,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -2154,7 +2270,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -2178,7 +2294,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -2202,7 +2318,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2226,12 +2342,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2244,13 +2360,13 @@
         <v>125</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2274,7 +2390,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -2298,7 +2414,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -2322,7 +2438,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -2346,7 +2462,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -2370,7 +2486,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -2394,7 +2510,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -2418,7 +2534,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -2442,7 +2558,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -2466,7 +2582,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -2490,7 +2606,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -2514,7 +2630,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -2538,7 +2654,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -2562,7 +2678,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>115</v>
       </c>
@@ -2586,7 +2702,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -2610,7 +2726,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -2634,7 +2750,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -2658,7 +2774,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>119</v>
       </c>
@@ -2682,13 +2798,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="B32" s="9"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="9"/>
-    </row>
-    <row r="35" spans="2:2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="8"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
   </sheetData>
@@ -2699,335 +2815,335 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
     <col min="3" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="99.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="99.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="8">
+        <v>167</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="8">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="8">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="8">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="8">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="8">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="8">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="8">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="8">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
         <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="8">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
         <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="8">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="8">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
         <v>10</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="8">
+      <c r="B15" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
         <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="8">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
         <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="8">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
         <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="8">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
         <v>14</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="8">
+      <c r="B19" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
         <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="8">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
         <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="8">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
         <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="8">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="8">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
         <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="8">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
         <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="8">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
         <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="8">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
         <v>22</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="8">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
         <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="8">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
         <v>24</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
commit with error after attempting to create an extension in the spreadsheet.
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9121 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26606"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/build/guides/daf2/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2970" yWindow="4215" windowWidth="25260" windowHeight="3885" activeTab="3"/>
+    <workbookView xWindow="28800" yWindow="-8420" windowWidth="25600" windowHeight="20480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
-  <calcPr calcId="125725" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -640,8 +645,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1034,32 +1039,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" customWidth="1"/>
-    <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" customWidth="1"/>
+    <col min="8" max="8" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.5" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="57" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1106,7 +1111,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1196,7 +1201,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1233,7 +1238,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1267,7 +1272,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75">
+    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1301,7 +1306,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75">
+    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1338,7 +1343,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75">
+    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1383,7 +1388,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75">
+    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1425,7 +1430,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75">
+    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1470,7 +1475,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75">
+    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1501,7 +1506,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75">
+    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1543,7 +1548,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75">
+    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1584,7 +1589,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75">
+    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1626,7 +1631,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75">
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1657,7 +1662,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75">
+    <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1699,7 +1704,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75">
+    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1741,7 +1746,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75">
+    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1783,7 +1788,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75">
+    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1825,7 +1830,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75">
+    <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1867,7 +1872,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75">
+    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1909,7 +1914,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75">
+    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1951,7 +1956,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75">
+    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1993,7 +1998,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75">
+    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -2035,7 +2040,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75">
+    <row r="25" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -2077,7 +2082,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75">
+    <row r="28" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
         <v>116</v>
       </c>
@@ -2106,7 +2111,7 @@
         <v>core-medicationdispense</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75">
+    <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
         <v>116</v>
       </c>
@@ -2135,7 +2140,7 @@
         <v>core-medicationadministration</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>115</v>
       </c>
@@ -2171,20 +2176,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>173</v>
       </c>
@@ -2192,7 +2197,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -2200,7 +2205,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>172</v>
       </c>
@@ -2208,7 +2213,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>175</v>
       </c>
@@ -2216,12 +2221,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>171</v>
       </c>
@@ -2229,7 +2234,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>183</v>
       </c>
@@ -2237,7 +2242,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>184</v>
       </c>
@@ -2251,37 +2256,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:J24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
     <col min="3" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="60" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" customWidth="1"/>
-    <col min="7" max="8" width="36.7109375" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="8" width="36.6640625" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -2310,7 +2315,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2339,7 +2344,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-ndfrt.xml</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2368,7 +2373,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-rxnorm.xml</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -2397,7 +2402,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-sct.xml</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2426,7 +2431,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-unii.xml</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>1</v>
       </c>
@@ -2454,11 +2459,11 @@
         <v>valueset-daf-core-substance</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6:I7" si="3">"http://hl7.org/fhir/daf/"&amp;G6</f>
+        <f t="shared" ref="I6" si="3">"http://hl7.org/fhir/daf/"&amp;G6</f>
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance.xml</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -2490,7 +2495,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-race.xml</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -2498,7 +2503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>5</v>
       </c>
@@ -2514,7 +2519,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>6</v>
       </c>
@@ -2522,7 +2527,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>7</v>
       </c>
@@ -2530,7 +2535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>8</v>
       </c>
@@ -2538,7 +2543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>9</v>
       </c>
@@ -2546,7 +2551,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>10</v>
       </c>
@@ -2554,7 +2559,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>11</v>
       </c>
@@ -2562,7 +2567,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>12</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>13</v>
       </c>
@@ -2578,7 +2583,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>14</v>
       </c>
@@ -2586,7 +2591,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>15</v>
       </c>
@@ -2594,7 +2599,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>16</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>17</v>
       </c>
@@ -2610,7 +2615,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -2618,7 +2623,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>19</v>
       </c>
@@ -2626,7 +2631,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>20</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>21</v>
       </c>
@@ -2642,7 +2647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>22</v>
       </c>
@@ -2650,7 +2655,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>23</v>
       </c>
@@ -2658,7 +2663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>24</v>
       </c>
@@ -2666,17 +2671,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>35</v>
       </c>
@@ -2687,24 +2692,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>190</v>
       </c>
@@ -2724,7 +2729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>56</v>
       </c>
@@ -2741,7 +2746,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -2774,7 +2779,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -2807,7 +2812,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -2840,7 +2845,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -2873,7 +2878,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2906,7 +2911,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -2939,7 +2944,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -2972,7 +2977,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -3005,7 +3010,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -3038,7 +3043,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -3071,7 +3076,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -3104,7 +3109,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -3137,7 +3142,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -3161,7 +3166,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -3185,7 +3190,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -3218,7 +3223,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="b">
         <v>1</v>
       </c>
@@ -3251,7 +3256,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="b">
         <v>1</v>
       </c>
@@ -3284,7 +3289,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -3317,7 +3322,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="b">
         <v>1</v>
       </c>
@@ -3350,7 +3355,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -3383,7 +3388,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -3416,7 +3421,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -3449,7 +3454,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="b">
         <v>1</v>
       </c>
@@ -3482,7 +3487,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="b">
         <v>1</v>
       </c>
@@ -3515,28 +3520,24 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="35" spans="4:5">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="4:5">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="38" spans="4:5">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J26">
-    <filterColumn colId="3"/>
-    <filterColumn colId="4"/>
-    <filterColumn colId="5"/>
-  </autoFilter>
+  <autoFilter ref="A1:J26"/>
   <sortState ref="E3:E26">
     <sortCondition ref="E3"/>
   </sortState>

</xml_diff>

<commit_message>
update to daf after adding value set and partial extension to patient
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9130 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/build/guides/daf2/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="-2970" yWindow="4215" windowWidth="25260" windowHeight="3885" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
-  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="125725" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="203">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -640,22 +635,13 @@
   </si>
   <si>
     <t>spreadsheet reference</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>task</t>
-  </si>
-  <si>
-    <t>dragon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1048,32 +1034,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" customWidth="1"/>
-    <col min="8" max="8" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.5" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="57" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1120,7 +1106,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1165,7 +1151,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1210,7 +1196,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1247,7 +1233,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1281,7 +1267,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1315,7 +1301,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1352,7 +1338,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1397,7 +1383,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1439,7 +1425,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1484,7 +1470,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1515,7 +1501,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1557,7 +1543,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1598,7 +1584,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1640,7 +1626,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1671,7 +1657,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1713,7 +1699,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1755,7 +1741,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15.75">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1797,7 +1783,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1839,7 +1825,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1881,7 +1867,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1923,7 +1909,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1965,7 +1951,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="15.75">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -2007,7 +1993,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="15.75">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -2049,7 +2035,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="15.75">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -2091,7 +2077,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15.75">
       <c r="B28" s="6" t="s">
         <v>116</v>
       </c>
@@ -2120,7 +2106,7 @@
         <v>core-medicationdispense</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="15.75">
       <c r="B29" s="6" t="s">
         <v>116</v>
       </c>
@@ -2149,7 +2135,7 @@
         <v>core-medicationadministration</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15">
       <c r="B30" t="s">
         <v>115</v>
       </c>
@@ -2173,42 +2159,6 @@
       <c r="N30" t="str">
         <f t="shared" si="4"/>
         <v>core-</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" t="s">
-        <v>205</v>
-      </c>
-      <c r="H33" t="s">
-        <v>203</v>
-      </c>
-      <c r="I33" t="s">
-        <v>204</v>
-      </c>
-      <c r="J33" t="s">
-        <v>203</v>
-      </c>
-      <c r="K33" t="str">
-        <f t="shared" ref="K33" si="5">I33&amp;"-daf-core-profile-spreadsheet.xml"</f>
-        <v>task-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L33" t="str">
-        <f t="shared" ref="L33" si="6">I33&amp;"-daf-core"</f>
-        <v>task-daf-core</v>
-      </c>
-      <c r="M33" t="str">
-        <f t="shared" ref="M33" si="7">"daf-"&amp;N33</f>
-        <v>daf-core-task</v>
-      </c>
-      <c r="N33" t="str">
-        <f t="shared" ref="N33" si="8">"core-"&amp;I33</f>
-        <v>core-task</v>
-      </c>
-      <c r="O33" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2221,20 +2171,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>173</v>
       </c>
@@ -2242,7 +2192,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -2250,7 +2200,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
         <v>172</v>
       </c>
@@ -2258,7 +2208,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
         <v>175</v>
       </c>
@@ -2266,12 +2216,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>171</v>
       </c>
@@ -2279,7 +2229,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
         <v>183</v>
       </c>
@@ -2287,7 +2237,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
         <v>184</v>
       </c>
@@ -2301,37 +2251,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="60" customWidth="1"/>
-    <col min="6" max="6" width="31.5" customWidth="1"/>
-    <col min="7" max="8" width="36.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
+    <col min="7" max="8" width="36.7109375" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -2360,7 +2310,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2389,7 +2339,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-ndfrt.xml</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2418,7 +2368,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-rxnorm.xml</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -2447,7 +2397,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-sct.xml</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2476,7 +2426,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-unii.xml</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>1</v>
       </c>
@@ -2504,11 +2454,11 @@
         <v>valueset-daf-core-substance</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6" si="3">"http://hl7.org/fhir/daf/"&amp;G6</f>
+        <f t="shared" ref="I6:I7" si="3">"http://hl7.org/fhir/daf/"&amp;G6</f>
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance.xml</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -2540,7 +2490,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-race.xml</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -2548,7 +2498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -2556,7 +2506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>5</v>
       </c>
@@ -2564,7 +2514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>6</v>
       </c>
@@ -2572,7 +2522,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>7</v>
       </c>
@@ -2580,7 +2530,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>8</v>
       </c>
@@ -2588,7 +2538,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>9</v>
       </c>
@@ -2596,7 +2546,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>10</v>
       </c>
@@ -2604,7 +2554,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>11</v>
       </c>
@@ -2612,7 +2562,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="8">
         <v>12</v>
       </c>
@@ -2620,7 +2570,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="8">
         <v>13</v>
       </c>
@@ -2628,7 +2578,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="8">
         <v>14</v>
       </c>
@@ -2636,7 +2586,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="8">
         <v>15</v>
       </c>
@@ -2644,7 +2594,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="8">
         <v>16</v>
       </c>
@@ -2652,7 +2602,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="8">
         <v>17</v>
       </c>
@@ -2660,7 +2610,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -2668,7 +2618,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="8">
         <v>19</v>
       </c>
@@ -2676,7 +2626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="8">
         <v>20</v>
       </c>
@@ -2684,7 +2634,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="8">
         <v>21</v>
       </c>
@@ -2692,7 +2642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="8">
         <v>22</v>
       </c>
@@ -2700,7 +2650,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="8">
         <v>23</v>
       </c>
@@ -2708,7 +2658,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="8">
         <v>24</v>
       </c>
@@ -2716,17 +2666,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="B32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2">
       <c r="B33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
         <v>35</v>
       </c>
@@ -2737,24 +2687,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="68.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>190</v>
       </c>
@@ -2774,7 +2724,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="B2" t="s">
         <v>56</v>
       </c>
@@ -2791,7 +2741,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -2824,7 +2774,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -2857,7 +2807,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -2890,7 +2840,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -2923,7 +2873,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2956,7 +2906,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -2989,7 +2939,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -3022,7 +2972,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -3055,7 +3005,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -3088,7 +3038,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -3121,7 +3071,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -3154,7 +3104,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -3187,7 +3137,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -3211,7 +3161,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -3235,7 +3185,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -3268,7 +3218,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" t="b">
         <v>1</v>
       </c>
@@ -3301,7 +3251,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" t="b">
         <v>1</v>
       </c>
@@ -3334,7 +3284,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -3367,7 +3317,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" t="b">
         <v>1</v>
       </c>
@@ -3400,7 +3350,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -3433,7 +3383,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -3466,7 +3416,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -3499,7 +3449,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" t="b">
         <v>1</v>
       </c>
@@ -3532,7 +3482,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" t="b">
         <v>1</v>
       </c>
@@ -3565,24 +3515,28 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:5">
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:5">
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:5">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J26"/>
+  <autoFilter ref="A1:J26">
+    <filterColumn colId="3"/>
+    <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
+  </autoFilter>
   <sortState ref="E3:E26">
     <sortCondition ref="E3"/>
   </sortState>

</xml_diff>

<commit_message>
update to daf core patient , add care team
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9153 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-2970" yWindow="4215" windowWidth="25260" windowHeight="3885" activeTab="3"/>
+    <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
-  <calcPr calcId="125725" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="180">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -34,9 +34,6 @@
     <t>AllergyIntolerance</t>
   </si>
   <si>
-    <t>daf-core-allergyintolerance</t>
-  </si>
-  <si>
     <t>CareTeam</t>
   </si>
   <si>
@@ -52,63 +49,6 @@
     <t>observation-daf-core-resultsv2</t>
   </si>
   <si>
-    <t>daf-core-careplan</t>
-  </si>
-  <si>
-    <t>daf-core-careteam</t>
-  </si>
-  <si>
-    <t>daf-core-condition</t>
-  </si>
-  <si>
-    <t>daf-core-diagnosticreport</t>
-  </si>
-  <si>
-    <t>daf-core-goals</t>
-  </si>
-  <si>
-    <t>daf-core-immunization</t>
-  </si>
-  <si>
-    <t>daf-core-location</t>
-  </si>
-  <si>
-    <t>daf-core-medication</t>
-  </si>
-  <si>
-    <t>daf-core-medicationadministration</t>
-  </si>
-  <si>
-    <t>daf-core-medicationdispense</t>
-  </si>
-  <si>
-    <t>daf-core-medicationorder</t>
-  </si>
-  <si>
-    <t>daf-core-medicationstatement</t>
-  </si>
-  <si>
-    <t>daf-core-observation-results</t>
-  </si>
-  <si>
-    <t>daf-core-observation-resultsv2</t>
-  </si>
-  <si>
-    <t>daf-core-observation-smokingstatus</t>
-  </si>
-  <si>
-    <t>daf-core-observation-vitalsigns</t>
-  </si>
-  <si>
-    <t>daf-core-organization</t>
-  </si>
-  <si>
-    <t>daf-core-patient</t>
-  </si>
-  <si>
-    <t>daf-core-practitioner</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -172,15 +112,9 @@
     <t>Conformance</t>
   </si>
   <si>
-    <t>daf-core-conformance</t>
-  </si>
-  <si>
     <t>DocumentReference</t>
   </si>
   <si>
-    <t>daf-core-documentreference</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -232,9 +166,6 @@
     <t xml:space="preserve">[ Observation-Results ](observation-daf-core-results.html) </t>
   </si>
   <si>
-    <t xml:space="preserve">[ Observation-Resultsv2 ](observation-daf-core-resultsv2.html) </t>
-  </si>
-  <si>
     <t xml:space="preserve">[ Observation-Smokingstatus ](observation-daf-core-smokingstatus.html) </t>
   </si>
   <si>
@@ -388,9 +319,6 @@
     <t>Device-UDI</t>
   </si>
   <si>
-    <t>daf-core-device-udi</t>
-  </si>
-  <si>
     <t xml:space="preserve">[ Device-UDI](device-daf-core-udi.html) </t>
   </si>
   <si>
@@ -583,9 +511,6 @@
     <t>-mappings.html</t>
   </si>
   <si>
-    <t>Created- but not working</t>
-  </si>
-  <si>
     <t>device</t>
   </si>
   <si>
@@ -635,6 +560,12 @@
   </si>
   <si>
     <t>spreadsheet reference</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>[Endpoint](endpoint-daf-core.html)</t>
   </si>
 </sst>
 </file>
@@ -1037,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1061,49 +992,49 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75">
@@ -1111,22 +1042,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
@@ -1148,7 +1079,7 @@
         <v>core-allergyintolerance</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75">
@@ -1156,25 +1087,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="H3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="J3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K30" si="0">I3&amp;"-daf-core-profile-spreadsheet.xml"</f>
@@ -1193,7 +1124,7 @@
         <v>core-careplan</v>
       </c>
       <c r="O3" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75">
@@ -1201,25 +1132,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" t="s">
         <v>95</v>
       </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>185</v>
-      </c>
-      <c r="G4" t="s">
-        <v>118</v>
-      </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
@@ -1229,8 +1160,16 @@
         <f t="shared" si="1"/>
         <v>careteam-daf-core</v>
       </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4" si="4">"daf-"&amp;N4</f>
+        <v>daf-core-careteam</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4" si="5">"core-"&amp;I4</f>
+        <v>core-careteam</v>
+      </c>
       <c r="O4" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
@@ -1238,22 +1177,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
@@ -1264,7 +1203,7 @@
         <v>conformance-daf-core</v>
       </c>
       <c r="O5" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
@@ -1272,33 +1211,33 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="G6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
         <v>118</v>
       </c>
-      <c r="H6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>documentreference-daf-core-profile-spreadsheet.xml</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>documentreference-daf-core</v>
+      </c>
+      <c r="O6" t="s">
         <v>142</v>
-      </c>
-      <c r="J6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="0"/>
-        <v>documentreference-daf-core-profile-spreadsheet.xml</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="1"/>
-        <v>documentreference-daf-core</v>
-      </c>
-      <c r="O6" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
@@ -1306,25 +1245,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="I7" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="J7" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
@@ -1335,7 +1274,7 @@
         <v>endpoint-daf-core</v>
       </c>
       <c r="O7" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
@@ -1343,25 +1282,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="H8" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="I8" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="J8" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
@@ -1380,7 +1319,7 @@
         <v>core-goal</v>
       </c>
       <c r="O8" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
@@ -1388,22 +1327,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
@@ -1422,7 +1361,7 @@
         <v>core-immunization</v>
       </c>
       <c r="O9" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
@@ -1430,25 +1369,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="G10" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="I10" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
@@ -1467,7 +1406,7 @@
         <v>core-device</v>
       </c>
       <c r="O10" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
@@ -1475,19 +1414,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="1"/>
@@ -1498,7 +1437,7 @@
         <v>daf-</v>
       </c>
       <c r="O11" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75">
@@ -1506,22 +1445,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
@@ -1540,7 +1479,7 @@
         <v>core-diagnosticreport</v>
       </c>
       <c r="O12" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75">
@@ -1548,25 +1487,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="I13" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="J13" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="K13" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="1"/>
@@ -1581,7 +1520,7 @@
         <v>core-resultobs</v>
       </c>
       <c r="O13" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75">
@@ -1589,22 +1528,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="J14" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
@@ -1623,7 +1562,7 @@
         <v>core-location</v>
       </c>
       <c r="O14" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75">
@@ -1631,19 +1570,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="1"/>
@@ -1654,7 +1593,7 @@
         <v>daf-</v>
       </c>
       <c r="O15" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75">
@@ -1662,22 +1601,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H16" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="I16" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="J16" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
@@ -1696,7 +1635,7 @@
         <v>core-medicationorder</v>
       </c>
       <c r="O16" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75">
@@ -1704,22 +1643,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H17" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="J17" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
@@ -1738,7 +1677,7 @@
         <v>core-medicationstatement</v>
       </c>
       <c r="O17" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75">
@@ -1746,22 +1685,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H18" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="I18" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="J18" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
@@ -1780,7 +1719,7 @@
         <v>core-medication</v>
       </c>
       <c r="O18" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75">
@@ -1788,22 +1727,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H19" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="J19" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
@@ -1822,7 +1761,7 @@
         <v>core-organization</v>
       </c>
       <c r="O19" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75">
@@ -1830,22 +1769,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="H20" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="J20" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
@@ -1864,7 +1803,7 @@
         <v>core-patient</v>
       </c>
       <c r="O20" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75">
@@ -1872,22 +1811,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H21" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="J21" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
@@ -1906,7 +1845,7 @@
         <v>core-pract</v>
       </c>
       <c r="O21" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75">
@@ -1914,22 +1853,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H22" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="I22" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="J22" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="0"/>
@@ -1948,7 +1887,7 @@
         <v>core-condition</v>
       </c>
       <c r="O22" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75">
@@ -1956,22 +1895,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H23" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="I23" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="J23" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
@@ -1990,7 +1929,7 @@
         <v>core-procedure</v>
       </c>
       <c r="O23" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75">
@@ -1998,22 +1937,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H24" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="I24" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="J24" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="0"/>
@@ -2032,7 +1971,7 @@
         <v>core-smokingstatus</v>
       </c>
       <c r="O24" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75">
@@ -2040,22 +1979,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="I25" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="J25" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="0"/>
@@ -2074,90 +2013,90 @@
         <v>core-vitalsigns</v>
       </c>
       <c r="O25" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75">
       <c r="B28" s="6" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="H28" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="I28" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="J28" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="0"/>
         <v>medicationdispense-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-medicationdispense</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" ref="N28:N30" si="4">"core-"&amp;I28</f>
+        <f t="shared" ref="N28:N30" si="6">"core-"&amp;I28</f>
         <v>core-medicationdispense</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75">
       <c r="B29" s="6" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="H29" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="I29" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="J29" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="0"/>
         <v>medicationadministration-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-medicationadministration</v>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>core-medicationadministration</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="B30" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="H30" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="J30" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
         <v>-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="L30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-</v>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>core-</v>
       </c>
     </row>
@@ -2186,63 +2125,63 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2266,7 +2205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:J24"/>
     </sheetView>
   </sheetViews>
@@ -2283,31 +2222,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2318,13 +2257,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G5" si="0">"ValueSet/"&amp;C2&amp;".xml"</f>
@@ -2347,13 +2286,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -2376,13 +2315,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="E4" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -2405,13 +2344,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="D5" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="E5" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -2434,16 +2373,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="G6" t="str">
         <f>"ValueSet/"&amp;C6&amp;".xml"</f>
@@ -2454,7 +2393,7 @@
         <v>valueset-daf-core-substance</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6:I7" si="3">"http://hl7.org/fhir/daf/"&amp;G6</f>
+        <f t="shared" ref="I6" si="3">"http://hl7.org/fhir/daf/"&amp;G6</f>
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance.xml</v>
       </c>
     </row>
@@ -2463,19 +2402,19 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="G7" t="str">
         <f>"ValueSet/"&amp;C7&amp;".xml"</f>
@@ -2495,7 +2434,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2503,7 +2442,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2511,7 +2450,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2519,7 +2458,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2527,7 +2466,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2535,7 +2474,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2543,7 +2482,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2551,7 +2490,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2559,7 +2498,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2567,7 +2506,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2575,7 +2514,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2583,7 +2522,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2591,7 +2530,7 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2599,7 +2538,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2607,7 +2546,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2615,7 +2554,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2623,7 +2562,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2631,7 +2570,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2639,7 +2578,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2647,7 +2586,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2655,7 +2594,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -2663,22 +2602,22 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="B32" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2690,8 +2629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2701,44 +2640,44 @@
     <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2746,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C3" t="str">
         <f>G3&amp;E3&amp;H3&amp;I3&amp;J3</f>
@@ -2759,19 +2698,20 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" t="s">
-        <v>2</v>
+        <v>57</v>
+      </c>
+      <c r="I3" t="str">
+        <f>"daf-core-"&amp;F3</f>
+        <v>daf-core-allergyintolerance</v>
       </c>
       <c r="J3" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2779,65 +2719,67 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C26" si="0">G4&amp;E4&amp;H4&amp;I4&amp;J4</f>
         <v>[CarePlan](daf-core-careplan.html)</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I26" si="1">"daf-core-"&amp;F4</f>
+        <v>daf-core-careplan</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>[CareTeam](daf-core-careteam.html)</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>[CareTeam](daf-core-careteam.html)</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>140</v>
-      </c>
-      <c r="G5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-careteam</v>
       </c>
       <c r="J5" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2845,32 +2787,33 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>[Condition](daf-core-condition.html)</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-condition</v>
       </c>
       <c r="J6" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2878,32 +2821,33 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>[Conformance](daf-core-conformance.html)</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-conformance</v>
+      </c>
+      <c r="J7" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>[Conformance](daf-core-conformance.html)</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2911,32 +2855,33 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>[Device-UDI](daf-core-device-udi.html)</v>
+        <v>[Device-UDI](daf-core-device.html)</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" t="s">
-        <v>120</v>
+        <v>57</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-device</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2944,32 +2889,33 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>[DiagnosticReport-Results](daf-core-diagnosticreport.html)</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
+        <v>57</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-diagnosticreport</v>
       </c>
       <c r="J9" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2977,32 +2923,33 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>[DocumentReference](daf-core-documentreference.html)</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-documentreference</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3010,32 +2957,33 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>179</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>[Endpoint](daf-core-goals.html)</v>
+        <v>[Endpoint](daf-core-endpoint.html)</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F11" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="G11" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11" t="s">
-        <v>12</v>
+        <v>57</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-endpoint</v>
       </c>
       <c r="J11" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3043,32 +2991,33 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>[Goal](daf-core-immunization.html)</v>
+        <v>[Goal](daf-core-goal.html)</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="E12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="F12" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" t="s">
-        <v>13</v>
+        <v>57</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-goal</v>
       </c>
       <c r="J12" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3076,32 +3025,33 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>[Immunization](daf-core-location.html)</v>
+        <v>[Immunization](daf-core-immunization.html)</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
+        <v>57</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-immunization</v>
       </c>
       <c r="J13" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3109,32 +3059,33 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>[Location](daf-core-medication.html)</v>
+        <v>[Location](daf-core-location.html)</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" t="s">
-        <v>15</v>
+        <v>57</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-location</v>
       </c>
       <c r="J14" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3142,23 +3093,24 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>[](daf-core-medicationadministration.html)</v>
+        <v>[](daf-core-.html)</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" t="s">
-        <v>16</v>
+        <v>57</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-</v>
       </c>
       <c r="J15" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3166,23 +3118,24 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>[](daf-core-medicationdispense.html)</v>
+        <v>[](daf-core-.html)</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H16" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" t="s">
-        <v>17</v>
+        <v>57</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-</v>
       </c>
       <c r="J16" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3190,32 +3143,33 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>[Medication](daf-core-medicationorder.html)</v>
+        <v>[Medication](daf-core-medication.html)</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="G17" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-medication</v>
       </c>
       <c r="J17" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3223,32 +3177,33 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>[MedicationOrder](daf-core-medicationstatement.html)</v>
+        <v>[MedicationOrder](daf-core-medicationorder.html)</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" t="s">
-        <v>19</v>
+        <v>57</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-medicationorder</v>
       </c>
       <c r="J18" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3256,32 +3211,33 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>[MedicationStatement](daf-core-observation-results.html)</v>
+        <v>[MedicationStatement](daf-core-medicationstatement.html)</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" t="s">
-        <v>20</v>
+        <v>57</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-medicationstatement</v>
       </c>
       <c r="J19" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3289,32 +3245,33 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>[Observation-Results](daf-core-observation-resultsv2.html)</v>
+        <v>[Observation-Results](daf-core-resultobs.html)</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H20" t="s">
-        <v>80</v>
-      </c>
-      <c r="I20" t="s">
-        <v>21</v>
+        <v>57</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-resultobs</v>
       </c>
       <c r="J20" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3322,32 +3279,33 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>[Observation-Smokingstatus](daf-core-observation-smokingstatus.html)</v>
+        <v>[Observation-Smokingstatus](daf-core-smokingstatus.html)</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="G21" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
-      </c>
-      <c r="I21" t="s">
-        <v>22</v>
+        <v>57</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-smokingstatus</v>
       </c>
       <c r="J21" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -3355,32 +3313,33 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>[Observation-Vitalsigns](daf-core-observation-vitalsigns.html)</v>
+        <v>[Observation-Vitalsigns](daf-core-vitalsigns.html)</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="G22" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H22" t="s">
-        <v>80</v>
-      </c>
-      <c r="I22" t="s">
-        <v>23</v>
+        <v>57</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-vitalsigns</v>
       </c>
       <c r="J22" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -3388,32 +3347,33 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>[Organization](daf-core-organization.html)</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="G23" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H23" t="s">
-        <v>80</v>
-      </c>
-      <c r="I23" t="s">
-        <v>24</v>
+        <v>57</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-organization</v>
       </c>
       <c r="J23" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3421,32 +3381,33 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>[Patient](daf-core-patient.html)</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="G24" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H24" t="s">
-        <v>80</v>
-      </c>
-      <c r="I24" t="s">
-        <v>25</v>
+        <v>57</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-patient</v>
       </c>
       <c r="J24" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -3454,32 +3415,33 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>[Practitioner](daf-core-practitioner.html)</v>
+        <v>[Practitioner](daf-core-pract.html)</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H25" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" t="s">
-        <v>26</v>
+        <v>57</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-pract</v>
       </c>
       <c r="J25" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -3487,32 +3449,33 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>[Procedure](daf-core-practitioner.html)</v>
+        <v>[Procedure](daf-core-procedure.html)</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F26" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="G26" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="H26" t="s">
-        <v>80</v>
-      </c>
-      <c r="I26" t="s">
-        <v>26</v>
+        <v>57</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-procedure</v>
       </c>
       <c r="J26" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:10">

</xml_diff>

<commit_message>
updated profiles to match argo, new value set
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9188 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FHIR_Build\guides\daf2\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885" activeTab="4"/>
+    <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
-  <calcPr calcId="125725" refMode="R1C1"/>
+  <calcPr calcId="171027" refMode="R1C1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="182">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -541,9 +546,6 @@
     <t>canonical-url</t>
   </si>
   <si>
-    <t>completed</t>
-  </si>
-  <si>
     <t>review vocab get gg to fix rendering</t>
   </si>
   <si>
@@ -566,13 +568,22 @@
   </si>
   <si>
     <t>[Endpoint](endpoint-daf-core.html)</t>
+  </si>
+  <si>
+    <t>Quick review</t>
+  </si>
+  <si>
+    <t>BAM: Ready for QA</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: Text Summary, and html guidance is broken. Value set hook in for Careplan.text.status isn't working</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -965,22 +976,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="62.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="37.42578125" customWidth="1"/>
     <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
@@ -990,7 +1001,7 @@
     <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -1037,7 +1048,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1048,10 +1059,13 @@
         <v>69</v>
       </c>
       <c r="D2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" t="s">
         <v>171</v>
-      </c>
-      <c r="F2" t="s">
-        <v>172</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>1</v>
@@ -1082,7 +1096,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1093,7 +1107,10 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="G3" t="s">
         <v>95</v>
@@ -1127,7 +1144,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1138,7 +1155,7 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G4" t="s">
         <v>95</v>
@@ -1172,7 +1189,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1206,7 +1223,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75">
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1240,7 +1257,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75">
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1277,7 +1294,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75">
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1322,7 +1339,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75">
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1364,7 +1381,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75">
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1409,7 +1426,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75">
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1440,7 +1457,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75">
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1482,7 +1499,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75">
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1523,7 +1540,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75">
+    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1565,7 +1582,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75">
+    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1596,7 +1613,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75">
+    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1638,7 +1655,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75">
+    <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1680,7 +1697,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75">
+    <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1722,7 +1739,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75">
+    <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1764,7 +1781,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75">
+    <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1806,7 +1823,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75">
+    <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1848,7 +1865,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75">
+    <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1890,7 +1907,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75">
+    <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1932,7 +1949,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75">
+    <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -1974,7 +1991,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75">
+    <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -2016,7 +2033,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75">
+    <row r="28" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>93</v>
       </c>
@@ -2045,7 +2062,7 @@
         <v>core-medicationdispense</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75">
+    <row r="29" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>93</v>
       </c>
@@ -2074,7 +2091,7 @@
         <v>core-medicationadministration</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>92</v>
       </c>
@@ -2110,20 +2127,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -2131,7 +2148,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -2139,7 +2156,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>148</v>
       </c>
@@ -2147,7 +2164,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>151</v>
       </c>
@@ -2155,12 +2172,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -2168,7 +2185,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>159</v>
       </c>
@@ -2176,7 +2193,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>160</v>
       </c>
@@ -2190,26 +2207,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
@@ -2220,7 +2237,7 @@
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2243,13 +2260,13 @@
         <v>169</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2278,7 +2295,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-ndfrt.xml</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2307,7 +2324,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-rxnorm.xml</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -2336,7 +2353,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-sct.xml</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2365,7 +2382,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-unii.xml</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>1</v>
       </c>
@@ -2397,7 +2414,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance.xml</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -2405,16 +2422,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" t="s">
         <v>173</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>174</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="13" t="s">
         <v>175</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>176</v>
       </c>
       <c r="G7" t="str">
         <f>"ValueSet/"&amp;C7&amp;".xml"</f>
@@ -2429,7 +2446,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-race.xml</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -2437,7 +2454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -2445,7 +2462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>5</v>
       </c>
@@ -2453,7 +2470,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>6</v>
       </c>
@@ -2461,7 +2478,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>7</v>
       </c>
@@ -2469,7 +2486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>8</v>
       </c>
@@ -2477,7 +2494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>9</v>
       </c>
@@ -2485,7 +2502,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>10</v>
       </c>
@@ -2493,7 +2510,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>11</v>
       </c>
@@ -2501,7 +2518,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>12</v>
       </c>
@@ -2509,7 +2526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>13</v>
       </c>
@@ -2517,7 +2534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>14</v>
       </c>
@@ -2525,7 +2542,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>15</v>
       </c>
@@ -2533,7 +2550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>16</v>
       </c>
@@ -2541,7 +2558,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>17</v>
       </c>
@@ -2549,7 +2566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -2557,7 +2574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>19</v>
       </c>
@@ -2565,7 +2582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>20</v>
       </c>
@@ -2573,7 +2590,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>21</v>
       </c>
@@ -2581,7 +2598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>22</v>
       </c>
@@ -2589,7 +2606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>23</v>
       </c>
@@ -2597,7 +2614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>24</v>
       </c>
@@ -2605,17 +2622,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>15</v>
       </c>
@@ -2626,14 +2643,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
@@ -2643,7 +2660,7 @@
     <col min="8" max="9" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -2663,7 +2680,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -2680,7 +2697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -2714,7 +2731,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -2748,7 +2765,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -2782,7 +2799,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -2816,7 +2833,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2850,7 +2867,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -2884,7 +2901,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -2918,7 +2935,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -2952,12 +2969,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -2986,7 +3003,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -3020,7 +3037,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -3054,7 +3071,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -3088,7 +3105,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -3113,7 +3130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -3138,7 +3155,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -3172,7 +3189,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>1</v>
       </c>
@@ -3206,7 +3223,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>1</v>
       </c>
@@ -3240,7 +3257,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -3274,7 +3291,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>1</v>
       </c>
@@ -3308,7 +3325,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -3342,7 +3359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -3376,7 +3393,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -3410,7 +3427,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>1</v>
       </c>
@@ -3444,7 +3461,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>1</v>
       </c>
@@ -3478,28 +3495,24 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="35" spans="4:5">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="4:5">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="38" spans="4:5">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J26">
-    <filterColumn colId="3"/>
-    <filterColumn colId="4"/>
-    <filterColumn colId="5"/>
-  </autoFilter>
+  <autoFilter ref="A1:J26"/>
   <sortState ref="E3:E26">
     <sortCondition ref="E3"/>
   </sortState>

</xml_diff>

<commit_message>
adjusted element cardinality, bindings. Value sets still need work.
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9189 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="184">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -396,9 +396,6 @@
     <t>medicationadministration</t>
   </si>
   <si>
-    <t>Initial</t>
-  </si>
-  <si>
     <t>created</t>
   </si>
   <si>
@@ -577,6 +574,15 @@
   </si>
   <si>
     <t>7/21/2016 bam: Text Summary, and html guidance is broken. Value set hook in for Careplan.text.status isn't working</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: Need value set for status, and roles</t>
+  </si>
+  <si>
+    <t>7/21/2016 BAM: Is race extension correct?</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: Need value set for status, and VaccineCode</t>
   </si>
 </sst>
 </file>
@@ -980,7 +986,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1051,7 @@
         <v>60</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1059,13 +1065,13 @@
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>1</v>
@@ -1093,7 +1099,7 @@
         <v>core-allergyintolerance</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -1107,10 +1113,10 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="G3" t="s">
         <v>95</v>
@@ -1141,7 +1147,7 @@
         <v>core-careplan</v>
       </c>
       <c r="O3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1155,7 +1161,10 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="F4" t="s">
+        <v>181</v>
       </c>
       <c r="G4" t="s">
         <v>95</v>
@@ -1186,7 +1195,7 @@
         <v>core-careteam</v>
       </c>
       <c r="O4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1220,7 +1229,7 @@
         <v>conformance-daf-core</v>
       </c>
       <c r="O5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1254,7 +1263,7 @@
         <v>documentreference-daf-core</v>
       </c>
       <c r="O6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1268,20 +1277,20 @@
         <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G7" t="s">
         <v>91</v>
       </c>
       <c r="H7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" t="s">
         <v>143</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>144</v>
       </c>
-      <c r="J7" t="s">
-        <v>145</v>
-      </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>endpoint-daf-core-profile-spreadsheet.xml</v>
@@ -1291,7 +1300,7 @@
         <v>endpoint-daf-core</v>
       </c>
       <c r="O7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1305,19 +1314,19 @@
         <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G8" t="s">
         <v>95</v>
       </c>
       <c r="H8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" t="s">
         <v>162</v>
       </c>
-      <c r="I8" t="s">
-        <v>163</v>
-      </c>
       <c r="J8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
@@ -1336,7 +1345,7 @@
         <v>core-goal</v>
       </c>
       <c r="O8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1350,7 +1359,10 @@
         <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="F9" t="s">
+        <v>183</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
@@ -1378,7 +1390,7 @@
         <v>core-immunization</v>
       </c>
       <c r="O9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1392,7 +1404,7 @@
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G10" t="s">
         <v>95</v>
@@ -1401,7 +1413,7 @@
         <v>96</v>
       </c>
       <c r="I10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J10" t="s">
         <v>8</v>
@@ -1423,7 +1435,7 @@
         <v>core-device</v>
       </c>
       <c r="O10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1437,7 +1449,7 @@
         <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>90</v>
@@ -1454,7 +1466,7 @@
         <v>daf-</v>
       </c>
       <c r="O11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1468,7 +1480,7 @@
         <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -1496,7 +1508,7 @@
         <v>core-diagnosticreport</v>
       </c>
       <c r="O12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1510,7 +1522,7 @@
         <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
@@ -1522,7 +1534,7 @@
         <v>26</v>
       </c>
       <c r="K13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="1"/>
@@ -1537,7 +1549,7 @@
         <v>core-resultobs</v>
       </c>
       <c r="O13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1551,7 +1563,7 @@
         <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H14" t="s">
         <v>12</v>
@@ -1579,7 +1591,7 @@
         <v>core-location</v>
       </c>
       <c r="O14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1593,7 +1605,7 @@
         <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>90</v>
@@ -1610,7 +1622,7 @@
         <v>daf-</v>
       </c>
       <c r="O15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1624,7 +1636,7 @@
         <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H16" t="s">
         <v>24</v>
@@ -1652,7 +1664,7 @@
         <v>core-medicationorder</v>
       </c>
       <c r="O16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1666,7 +1678,7 @@
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H17" t="s">
         <v>25</v>
@@ -1694,7 +1706,7 @@
         <v>core-medicationstatement</v>
       </c>
       <c r="O17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1708,7 +1720,7 @@
         <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H18" t="s">
         <v>13</v>
@@ -1736,7 +1748,7 @@
         <v>core-medication</v>
       </c>
       <c r="O18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1750,7 +1762,7 @@
         <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
@@ -1778,7 +1790,7 @@
         <v>core-organization</v>
       </c>
       <c r="O19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1792,7 +1804,10 @@
         <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>179</v>
+      </c>
+      <c r="F20" t="s">
+        <v>182</v>
       </c>
       <c r="H20" t="s">
         <v>19</v>
@@ -1820,7 +1835,7 @@
         <v>core-patient</v>
       </c>
       <c r="O20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1834,7 +1849,7 @@
         <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
@@ -1862,7 +1877,7 @@
         <v>core-pract</v>
       </c>
       <c r="O21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1876,7 +1891,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H22" t="s">
         <v>7</v>
@@ -1904,7 +1919,7 @@
         <v>core-condition</v>
       </c>
       <c r="O22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1918,7 +1933,7 @@
         <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H23" t="s">
         <v>21</v>
@@ -1946,7 +1961,7 @@
         <v>core-procedure</v>
       </c>
       <c r="O23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1960,7 +1975,7 @@
         <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H24" t="s">
         <v>16</v>
@@ -1988,7 +2003,7 @@
         <v>core-smokingstatus</v>
       </c>
       <c r="O24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2002,7 +2017,7 @@
         <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H25" t="s">
         <v>17</v>
@@ -2030,7 +2045,7 @@
         <v>core-vitalsigns</v>
       </c>
       <c r="O25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2142,63 +2157,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
         <v>149</v>
-      </c>
-      <c r="B1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2245,25 +2260,25 @@
         <v>98</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>124</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2274,13 +2289,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G5" si="0">"ValueSet/"&amp;C2&amp;".xml"</f>
@@ -2303,13 +2318,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -2332,13 +2347,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -2361,13 +2376,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -2390,16 +2405,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G6" t="str">
         <f>"ValueSet/"&amp;C6&amp;".xml"</f>
@@ -2422,16 +2437,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" t="s">
         <v>172</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>173</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="13" t="s">
         <v>174</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>175</v>
       </c>
       <c r="G7" t="str">
         <f>"ValueSet/"&amp;C7&amp;".xml"</f>
@@ -2662,19 +2677,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>99</v>
@@ -2885,7 +2900,7 @@
         <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G8" t="s">
         <v>56</v>
@@ -2974,20 +2989,20 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>[Endpoint](daf-core-endpoint.html)</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" t="s">
         <v>143</v>
-      </c>
-      <c r="F11" t="s">
-        <v>144</v>
       </c>
       <c r="G11" t="s">
         <v>56</v>
@@ -3015,13 +3030,13 @@
         <v>[Goal](daf-core-goal.html)</v>
       </c>
       <c r="D12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" t="s">
         <v>162</v>
-      </c>
-      <c r="E12" t="s">
-        <v>162</v>
-      </c>
-      <c r="F12" t="s">
-        <v>163</v>
       </c>
       <c r="G12" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
update to daf device value set bindings
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9192 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="185">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -585,7 +585,7 @@
     <t>7/21/2016 bam: Need value set for status, and VaccineCode</t>
   </si>
   <si>
-    <t>7/21/2016 BAM: No additional value sets required. Html needs work</t>
+    <t>7/21/2016 bam: No additional value sets required. Html needs work</t>
   </si>
 </sst>
 </file>
@@ -989,7 +989,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1410,10 @@
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>121</v>
+        <v>179</v>
+      </c>
+      <c r="F10" t="s">
+        <v>184</v>
       </c>
       <c r="G10" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
several DAF-core and daf research updates. Builds locally on prior build.
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9204 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -13,15 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
-    <sheet name="exampletypesformappng" sheetId="5" r:id="rId2"/>
-    <sheet name="Extensions" sheetId="3" r:id="rId3"/>
-    <sheet name="ValueSets" sheetId="4" r:id="rId4"/>
-    <sheet name="Profiles-links" sheetId="2" r:id="rId5"/>
+    <sheet name="DAF-Research-Updates" sheetId="6" r:id="rId2"/>
+    <sheet name="exampletypesformappng" sheetId="5" r:id="rId3"/>
+    <sheet name="Extensions" sheetId="3" r:id="rId4"/>
+    <sheet name="ValueSets" sheetId="4" r:id="rId5"/>
+    <sheet name="Profiles-links" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DAF-Research-Updates'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
   <calcPr calcId="171027" refMode="R1C1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="189">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -561,18 +564,12 @@
     <t>spreadsheet reference</t>
   </si>
   <si>
-    <t>Created</t>
-  </si>
-  <si>
     <t>[Endpoint](endpoint-daf-core.html)</t>
   </si>
   <si>
     <t>Quick review</t>
   </si>
   <si>
-    <t>7/21/2016 bam: Text Summary, and html guidance is broken. Value set hook in for Careplan.text.status isn't working</t>
-  </si>
-  <si>
     <t>7/21/2016 bam: Need value set for status, and roles</t>
   </si>
   <si>
@@ -589,6 +586,21 @@
   </si>
   <si>
     <t>7/21/2016 bam: Is race extension correct?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/21/2016 bam: Text Summary, and html guidance is broken. </t>
+  </si>
+  <si>
+    <t>DAF Research Profiles</t>
+  </si>
+  <si>
+    <t>Reuse core</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: Fixing to LOINC in code.system, and reference to pracitioner.</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: Reference to pracitioner may need to be fixed.</t>
   </si>
 </sst>
 </file>
@@ -654,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -685,6 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,7 +1005,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,10 +1084,10 @@
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
         <v>170</v>
@@ -1108,7 +1121,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1119,10 +1132,10 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G3" t="s">
         <v>95</v>
@@ -1167,10 +1180,10 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="F4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G4" t="s">
         <v>95</v>
@@ -1320,10 +1333,10 @@
         <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G8" t="s">
         <v>95</v>
@@ -1368,10 +1381,10 @@
         <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>182</v>
       </c>
       <c r="F9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
@@ -1413,10 +1426,10 @@
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G10" t="s">
         <v>95</v>
@@ -1457,12 +1470,6 @@
       <c r="B11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>121</v>
-      </c>
       <c r="H11" s="9" t="s">
         <v>90</v>
       </c>
@@ -1492,7 +1499,10 @@
         <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>181</v>
+      </c>
+      <c r="F12" t="s">
+        <v>187</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -1534,7 +1544,7 @@
         <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
@@ -1613,12 +1623,6 @@
       <c r="B15" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" t="s">
-        <v>121</v>
-      </c>
       <c r="H15" s="9" t="s">
         <v>90</v>
       </c>
@@ -1648,7 +1652,10 @@
         <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>181</v>
+      </c>
+      <c r="F16" t="s">
+        <v>188</v>
       </c>
       <c r="H16" t="s">
         <v>24</v>
@@ -1690,7 +1697,7 @@
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="H17" t="s">
         <v>25</v>
@@ -1732,7 +1739,7 @@
         <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="H18" t="s">
         <v>13</v>
@@ -1816,10 +1823,10 @@
         <v>69</v>
       </c>
       <c r="D20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" t="s">
         <v>183</v>
-      </c>
-      <c r="F20" t="s">
-        <v>185</v>
       </c>
       <c r="H20" t="s">
         <v>19</v>
@@ -2154,6 +2161,337 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="62.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="14">
+        <v>42573</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="14">
+        <v>42573</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -2233,7 +2571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2245,7 +2583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
@@ -2669,7 +3007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
@@ -3001,7 +3339,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
trimming daf to core
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9210 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -24,7 +24,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
   <calcPr calcId="171027" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="191">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -601,6 +600,12 @@
   </si>
   <si>
     <t>7/21/2016 bam: Reference to pracitioner may need to be fixed.</t>
+  </si>
+  <si>
+    <t>7/22/2016 bam: Needs NUCC code system and value set</t>
+  </si>
+  <si>
+    <t>Not created</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1010,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,6 +1232,9 @@
       <c r="C5" t="s">
         <v>75</v>
       </c>
+      <c r="D5" t="s">
+        <v>182</v>
+      </c>
       <c r="G5" t="s">
         <v>95</v>
       </c>
@@ -1261,6 +1269,9 @@
       <c r="C6" t="s">
         <v>75</v>
       </c>
+      <c r="D6" t="s">
+        <v>190</v>
+      </c>
       <c r="G6" t="s">
         <v>95</v>
       </c>
@@ -1295,6 +1306,9 @@
       <c r="C7" t="s">
         <v>75</v>
       </c>
+      <c r="D7" t="s">
+        <v>190</v>
+      </c>
       <c r="F7" t="s">
         <v>145</v>
       </c>
@@ -1781,7 +1795,7 @@
         <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
@@ -1868,7 +1882,10 @@
         <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>181</v>
+      </c>
+      <c r="F21" t="s">
+        <v>189</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
parsing daf down to daf-core and adding new value sets.
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9211 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="193">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -606,6 +606,12 @@
   </si>
   <si>
     <t>Not created</t>
+  </si>
+  <si>
+    <t>7/22/2016 bam: Need to add requirement that procedure.code is SNOMED or CPT with ICD10 allowed in translation</t>
+  </si>
+  <si>
+    <t>7/22/2016 bam: Value sets are stubs. Need to be cleaned up.</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1016,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,7 +1933,7 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="H22" t="s">
         <v>7</v>
@@ -1958,7 +1964,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1969,7 +1975,10 @@
         <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>181</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="H23" t="s">
         <v>21</v>
@@ -2011,7 +2020,7 @@
         <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="H24" t="s">
         <v>16</v>
@@ -2053,7 +2062,10 @@
         <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>181</v>
+      </c>
+      <c r="F25" t="s">
+        <v>192</v>
       </c>
       <c r="H25" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
new value sets and updates to daf-core profiles.
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9231 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="196">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -545,9 +545,6 @@
     <t>canonical-url</t>
   </si>
   <si>
-    <t>review vocab get gg to fix rendering</t>
-  </si>
-  <si>
     <t>daf-race</t>
   </si>
   <si>
@@ -612,6 +609,18 @@
   </si>
   <si>
     <t>7/22/2016 bam: Value sets are stubs. Need to be cleaned up.</t>
+  </si>
+  <si>
+    <t>Value sets</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>in build, not displaying</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -1013,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,19 +1034,21 @@
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="62.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="62.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.42578125" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="57" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -1051,40 +1062,44 @@
         <v>65</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1095,44 +1110,44 @@
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" t="str">
-        <f>I2&amp;"-daf-core-profile-spreadsheet.xml"</f>
+      <c r="K2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="str">
+        <f>K2&amp;"-daf-core-profile-spreadsheet.xml"</f>
         <v>allergyintolerance-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L2" t="str">
-        <f>I2&amp;"-daf-core"</f>
+      <c r="N2" t="str">
+        <f>K2&amp;"-daf-core"</f>
         <v>allergyintolerance-daf-core</v>
       </c>
-      <c r="M2" t="str">
-        <f>"daf-"&amp;N2</f>
+      <c r="O2" t="str">
+        <f>"daf-"&amp;P2</f>
         <v>daf-core-allergyintolerance</v>
       </c>
-      <c r="N2" t="str">
-        <f>"core-"&amp;I2</f>
+      <c r="P2" t="str">
+        <f>"core-"&amp;K2</f>
         <v>core-allergyintolerance</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1143,44 +1158,47 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" t="s">
         <v>95</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>115</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K30" si="0">I3&amp;"-daf-core-profile-spreadsheet.xml"</f>
+      <c r="K3" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M30" si="0">K3&amp;"-daf-core-profile-spreadsheet.xml"</f>
         <v>careplan-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L25" si="1">I3&amp;"-daf-core"</f>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N25" si="1">K3&amp;"-daf-core"</f>
         <v>careplan-daf-core</v>
       </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M30" si="2">"daf-"&amp;N3</f>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O30" si="2">"daf-"&amp;P3</f>
         <v>daf-core-careplan</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N25" si="3">"core-"&amp;I3</f>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P25" si="3">"core-"&amp;K3</f>
         <v>core-careplan</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1191,44 +1209,47 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F4" t="s">
-        <v>178</v>
-      </c>
-      <c r="G4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I4" t="s">
         <v>95</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>116</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
       </c>
-      <c r="K4" t="str">
+      <c r="K4" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" t="str">
         <f t="shared" si="0"/>
         <v>careteam-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L4" t="str">
+      <c r="N4" t="str">
         <f t="shared" si="1"/>
         <v>careteam-daf-core</v>
       </c>
-      <c r="M4" t="str">
-        <f t="shared" ref="M4" si="4">"daf-"&amp;N4</f>
+      <c r="O4" t="str">
+        <f t="shared" ref="O4" si="4">"daf-"&amp;P4</f>
         <v>daf-core-careteam</v>
       </c>
-      <c r="N4" t="str">
-        <f t="shared" ref="N4" si="5">"core-"&amp;I4</f>
+      <c r="P4" t="str">
+        <f t="shared" ref="P4" si="5">"core-"&amp;K4</f>
         <v>core-careteam</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1239,33 +1260,33 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
-      </c>
-      <c r="G5" t="s">
+        <v>181</v>
+      </c>
+      <c r="I5" t="s">
         <v>95</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>117</v>
       </c>
       <c r="J5" t="s">
         <v>27</v>
       </c>
-      <c r="K5" t="str">
+      <c r="K5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="str">
         <f t="shared" si="0"/>
         <v>conformance-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L5" t="str">
+      <c r="N5" t="str">
         <f t="shared" si="1"/>
         <v>conformance-daf-core</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1276,33 +1297,33 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G6" t="s">
+        <v>189</v>
+      </c>
+      <c r="I6" t="s">
         <v>95</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>118</v>
       </c>
       <c r="J6" t="s">
         <v>28</v>
       </c>
-      <c r="K6" t="str">
+      <c r="K6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="str">
         <f t="shared" si="0"/>
         <v>documentreference-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L6" t="str">
+      <c r="N6" t="str">
         <f t="shared" si="1"/>
         <v>documentreference-daf-core</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1313,36 +1334,36 @@
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F7" t="s">
+        <v>189</v>
+      </c>
+      <c r="H7" t="s">
         <v>145</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>91</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>142</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>143</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>144</v>
       </c>
-      <c r="K7" t="str">
+      <c r="M7" t="str">
         <f t="shared" si="0"/>
         <v>endpoint-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L7" t="str">
+      <c r="N7" t="str">
         <f t="shared" si="1"/>
         <v>endpoint-daf-core</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1353,44 +1374,47 @@
         <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F8" t="s">
         <v>180</v>
       </c>
-      <c r="G8" t="s">
+      <c r="E8" t="s">
+        <v>195</v>
+      </c>
+      <c r="H8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" t="s">
         <v>95</v>
-      </c>
-      <c r="H8" t="s">
-        <v>161</v>
-      </c>
-      <c r="I8" t="s">
-        <v>162</v>
       </c>
       <c r="J8" t="s">
         <v>161</v>
       </c>
-      <c r="K8" t="str">
+      <c r="K8" t="s">
+        <v>162</v>
+      </c>
+      <c r="L8" t="s">
+        <v>161</v>
+      </c>
+      <c r="M8" t="str">
         <f t="shared" si="0"/>
         <v>goal-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L8" t="str">
+      <c r="N8" t="str">
         <f t="shared" si="1"/>
         <v>goal-daf-core</v>
       </c>
-      <c r="M8" t="str">
+      <c r="O8" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-goal</v>
       </c>
-      <c r="N8" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="3"/>
         <v>core-goal</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1401,41 +1425,44 @@
         <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" t="s">
-        <v>179</v>
+        <v>180</v>
+      </c>
+      <c r="E9" t="s">
+        <v>194</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" t="s">
-        <v>105</v>
+        <v>178</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
       </c>
-      <c r="K9" t="str">
+      <c r="K9" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" t="str">
         <f t="shared" si="0"/>
         <v>immunization-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L9" t="str">
+      <c r="N9" t="str">
         <f t="shared" si="1"/>
         <v>immunization-daf-core</v>
       </c>
-      <c r="M9" t="str">
+      <c r="O9" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-immunization</v>
       </c>
-      <c r="N9" t="str">
+      <c r="P9" t="str">
         <f t="shared" si="3"/>
         <v>core-immunization</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1446,69 +1473,72 @@
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
-      </c>
-      <c r="F10" t="s">
         <v>180</v>
       </c>
-      <c r="G10" t="s">
+      <c r="E10" t="s">
+        <v>194</v>
+      </c>
+      <c r="H10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I10" t="s">
         <v>95</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>96</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>160</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>8</v>
       </c>
-      <c r="K10" t="str">
+      <c r="M10" t="str">
         <f t="shared" si="0"/>
         <v>device-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L10" t="str">
+      <c r="N10" t="str">
         <f t="shared" si="1"/>
         <v>device-daf-core</v>
       </c>
-      <c r="M10" t="str">
+      <c r="O10" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-device</v>
       </c>
-      <c r="N10" t="str">
+      <c r="P10" t="str">
         <f t="shared" si="3"/>
         <v>core-device</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>90</v>
-      </c>
       <c r="J11" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L11" t="str">
+      <c r="L11" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N11" t="str">
         <f t="shared" si="1"/>
         <v>-daf-core</v>
       </c>
-      <c r="M11" t="str">
+      <c r="O11" t="str">
         <f t="shared" si="2"/>
         <v>daf-</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1519,41 +1549,44 @@
         <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
-      </c>
-      <c r="F12" t="s">
-        <v>187</v>
+        <v>180</v>
+      </c>
+      <c r="E12" t="s">
+        <v>194</v>
       </c>
       <c r="H12" t="s">
+        <v>186</v>
+      </c>
+      <c r="J12" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>9</v>
       </c>
-      <c r="K12" t="str">
+      <c r="M12" t="str">
         <f t="shared" si="0"/>
         <v>diagnosticreport-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L12" t="str">
+      <c r="N12" t="str">
         <f t="shared" si="1"/>
         <v>diagnosticreport-daf-core</v>
       </c>
-      <c r="M12" t="str">
+      <c r="O12" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-diagnosticreport</v>
       </c>
-      <c r="N12" t="str">
+      <c r="P12" t="str">
         <f t="shared" si="3"/>
         <v>core-diagnosticreport</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1564,37 +1597,40 @@
         <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
-      </c>
-      <c r="H13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" t="s">
+        <v>194</v>
+      </c>
+      <c r="J13" t="s">
         <v>14</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>111</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>26</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>163</v>
       </c>
-      <c r="L13" t="str">
+      <c r="N13" t="str">
         <f t="shared" si="1"/>
         <v>resultobs-daf-core</v>
       </c>
-      <c r="M13" t="str">
+      <c r="O13" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-resultobs</v>
       </c>
-      <c r="N13" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="3"/>
         <v>core-resultobs</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1607,61 +1643,61 @@
       <c r="D14" t="s">
         <v>121</v>
       </c>
-      <c r="H14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" t="s">
-        <v>112</v>
-      </c>
       <c r="J14" t="s">
         <v>12</v>
       </c>
-      <c r="K14" t="str">
+      <c r="K14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" t="str">
         <f t="shared" si="0"/>
         <v>location-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L14" t="str">
+      <c r="N14" t="str">
         <f t="shared" si="1"/>
         <v>location-daf-core</v>
       </c>
-      <c r="M14" t="str">
+      <c r="O14" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-location</v>
       </c>
-      <c r="N14" t="str">
+      <c r="P14" t="str">
         <f t="shared" si="3"/>
         <v>core-location</v>
       </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>90</v>
-      </c>
       <c r="J15" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L15" t="str">
+      <c r="L15" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N15" t="str">
         <f t="shared" si="1"/>
         <v>-daf-core</v>
       </c>
-      <c r="M15" t="str">
+      <c r="O15" t="str">
         <f t="shared" si="2"/>
         <v>daf-</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1672,41 +1708,41 @@
         <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
-      </c>
-      <c r="F16" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="J16" t="s">
         <v>24</v>
       </c>
-      <c r="K16" t="str">
+      <c r="K16" t="s">
+        <v>103</v>
+      </c>
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" t="str">
         <f t="shared" si="0"/>
         <v>medicationorder-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L16" t="str">
+      <c r="N16" t="str">
         <f t="shared" si="1"/>
         <v>medicationorder-daf-core</v>
       </c>
-      <c r="M16" t="str">
+      <c r="O16" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-medicationorder</v>
       </c>
-      <c r="N16" t="str">
+      <c r="P16" t="str">
         <f t="shared" si="3"/>
         <v>core-medicationorder</v>
       </c>
-      <c r="O16" t="s">
+      <c r="Q16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1717,38 +1753,38 @@
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
-      </c>
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>109</v>
+        <v>180</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
       </c>
-      <c r="K17" t="str">
+      <c r="K17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="L17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" t="str">
         <f t="shared" si="0"/>
         <v>medicationstatement-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L17" t="str">
+      <c r="N17" t="str">
         <f t="shared" si="1"/>
         <v>medicationstatement-daf-core</v>
       </c>
-      <c r="M17" t="str">
+      <c r="O17" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-medicationstatement</v>
       </c>
-      <c r="N17" t="str">
+      <c r="P17" t="str">
         <f t="shared" si="3"/>
         <v>core-medicationstatement</v>
       </c>
-      <c r="O17" t="s">
+      <c r="Q17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1759,38 +1795,38 @@
         <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
-      </c>
-      <c r="H18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" t="s">
-        <v>108</v>
+        <v>180</v>
       </c>
       <c r="J18" t="s">
         <v>13</v>
       </c>
-      <c r="K18" t="str">
+      <c r="K18" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" t="str">
         <f t="shared" si="0"/>
         <v>medication-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L18" t="str">
+      <c r="N18" t="str">
         <f t="shared" si="1"/>
         <v>medication-daf-core</v>
       </c>
-      <c r="M18" t="str">
+      <c r="O18" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-medication</v>
       </c>
-      <c r="N18" t="str">
+      <c r="P18" t="str">
         <f t="shared" si="3"/>
         <v>core-medication</v>
       </c>
-      <c r="O18" t="s">
+      <c r="Q18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1801,38 +1837,38 @@
         <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
-      </c>
-      <c r="H19" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
       </c>
-      <c r="K19" t="str">
+      <c r="K19" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="L19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" t="str">
         <f t="shared" si="0"/>
         <v>organization-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L19" t="str">
+      <c r="N19" t="str">
         <f t="shared" si="1"/>
         <v>organization-daf-core</v>
       </c>
-      <c r="M19" t="str">
+      <c r="O19" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-organization</v>
       </c>
-      <c r="N19" t="str">
+      <c r="P19" t="str">
         <f t="shared" si="3"/>
         <v>core-organization</v>
       </c>
-      <c r="O19" t="s">
+      <c r="Q19" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1843,41 +1879,41 @@
         <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>181</v>
-      </c>
-      <c r="F20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="J20" t="s">
         <v>19</v>
       </c>
-      <c r="K20" t="str">
+      <c r="K20" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" t="str">
         <f t="shared" si="0"/>
         <v>patient-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L20" t="str">
+      <c r="N20" t="str">
         <f t="shared" si="1"/>
         <v>patient-daf-core</v>
       </c>
-      <c r="M20" t="str">
+      <c r="O20" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-patient</v>
       </c>
-      <c r="N20" t="str">
+      <c r="P20" t="str">
         <f t="shared" si="3"/>
         <v>core-patient</v>
       </c>
-      <c r="O20" t="s">
+      <c r="Q20" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1888,41 +1924,41 @@
         <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>181</v>
-      </c>
-      <c r="F21" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" t="s">
-        <v>114</v>
+        <v>188</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
       </c>
-      <c r="K21" t="str">
+      <c r="K21" t="s">
+        <v>114</v>
+      </c>
+      <c r="L21" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" t="str">
         <f t="shared" si="0"/>
         <v>pract-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L21" t="str">
+      <c r="N21" t="str">
         <f t="shared" si="1"/>
         <v>pract-daf-core</v>
       </c>
-      <c r="M21" t="str">
+      <c r="O21" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-pract</v>
       </c>
-      <c r="N21" t="str">
+      <c r="P21" t="str">
         <f t="shared" si="3"/>
         <v>core-pract</v>
       </c>
-      <c r="O21" t="s">
+      <c r="Q21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1933,38 +1969,38 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>181</v>
-      </c>
-      <c r="H22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" t="s">
-        <v>102</v>
+        <v>180</v>
       </c>
       <c r="J22" t="s">
         <v>7</v>
       </c>
-      <c r="K22" t="str">
+      <c r="K22" t="s">
+        <v>102</v>
+      </c>
+      <c r="L22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" t="str">
         <f t="shared" si="0"/>
         <v>condition-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L22" t="str">
+      <c r="N22" t="str">
         <f t="shared" si="1"/>
         <v>condition-daf-core</v>
       </c>
-      <c r="M22" t="str">
+      <c r="O22" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-condition</v>
       </c>
-      <c r="N22" t="str">
+      <c r="P22" t="str">
         <f t="shared" si="3"/>
         <v>core-condition</v>
       </c>
-      <c r="O22" t="s">
+      <c r="Q22" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1975,41 +2011,41 @@
         <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>181</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="H23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" t="s">
-        <v>106</v>
+        <v>180</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="J23" t="s">
         <v>21</v>
       </c>
-      <c r="K23" t="str">
+      <c r="K23" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" t="str">
         <f t="shared" si="0"/>
         <v>procedure-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L23" t="str">
+      <c r="N23" t="str">
         <f t="shared" si="1"/>
         <v>procedure-daf-core</v>
       </c>
-      <c r="M23" t="str">
+      <c r="O23" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-procedure</v>
       </c>
-      <c r="N23" t="str">
+      <c r="P23" t="str">
         <f t="shared" si="3"/>
         <v>core-procedure</v>
       </c>
-      <c r="O23" t="s">
+      <c r="Q23" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -2020,38 +2056,38 @@
         <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>181</v>
-      </c>
-      <c r="H24" t="s">
+        <v>180</v>
+      </c>
+      <c r="J24" t="s">
         <v>16</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>110</v>
       </c>
-      <c r="J24" t="s">
+      <c r="L24" t="s">
         <v>26</v>
       </c>
-      <c r="K24" t="str">
+      <c r="M24" t="str">
         <f t="shared" si="0"/>
         <v>smokingstatus-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L24" t="str">
+      <c r="N24" t="str">
         <f t="shared" si="1"/>
         <v>smokingstatus-daf-core</v>
       </c>
-      <c r="M24" t="str">
+      <c r="O24" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-smokingstatus</v>
       </c>
-      <c r="N24" t="str">
+      <c r="P24" t="str">
         <f t="shared" si="3"/>
         <v>core-smokingstatus</v>
       </c>
-      <c r="O24" t="s">
+      <c r="Q24" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -2062,127 +2098,127 @@
         <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F25" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="H25" t="s">
+        <v>191</v>
+      </c>
+      <c r="J25" t="s">
         <v>17</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>107</v>
       </c>
-      <c r="J25" t="s">
+      <c r="L25" t="s">
         <v>26</v>
       </c>
-      <c r="K25" t="str">
+      <c r="M25" t="str">
         <f t="shared" si="0"/>
         <v>vitalsigns-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L25" t="str">
+      <c r="N25" t="str">
         <f t="shared" si="1"/>
         <v>vitalsigns-daf-core</v>
       </c>
-      <c r="M25" t="str">
+      <c r="O25" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-vitalsigns</v>
       </c>
-      <c r="N25" t="str">
+      <c r="P25" t="str">
         <f t="shared" si="3"/>
         <v>core-vitalsigns</v>
       </c>
-      <c r="O25" t="s">
+      <c r="Q25" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H28" t="s">
-        <v>23</v>
-      </c>
-      <c r="I28" t="s">
-        <v>119</v>
-      </c>
       <c r="J28" t="s">
         <v>23</v>
       </c>
-      <c r="K28" t="str">
+      <c r="K28" t="s">
+        <v>119</v>
+      </c>
+      <c r="L28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" t="str">
         <f t="shared" si="0"/>
         <v>medicationdispense-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>5</v>
       </c>
-      <c r="M28" t="str">
+      <c r="O28" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-medicationdispense</v>
       </c>
-      <c r="N28" t="str">
-        <f t="shared" ref="N28:N30" si="6">"core-"&amp;I28</f>
+      <c r="P28" t="str">
+        <f t="shared" ref="P28:P30" si="6">"core-"&amp;K28</f>
         <v>core-medicationdispense</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" t="s">
-        <v>120</v>
-      </c>
       <c r="J29" t="s">
         <v>22</v>
       </c>
-      <c r="K29" t="str">
+      <c r="K29" t="s">
+        <v>120</v>
+      </c>
+      <c r="L29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M29" t="str">
         <f t="shared" si="0"/>
         <v>medicationadministration-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>4</v>
       </c>
-      <c r="M29" t="str">
+      <c r="O29" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-medicationadministration</v>
       </c>
-      <c r="N29" t="str">
+      <c r="P29" t="str">
         <f t="shared" si="6"/>
         <v>core-medicationadministration</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>92</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J30" t="s">
         <v>15</v>
       </c>
-      <c r="J30" t="s">
+      <c r="L30" t="s">
         <v>26</v>
       </c>
-      <c r="K30" t="str">
+      <c r="M30" t="str">
         <f t="shared" si="0"/>
         <v>-daf-core-profile-spreadsheet.xml</v>
       </c>
-      <c r="L30" t="s">
+      <c r="N30" t="s">
         <v>6</v>
       </c>
-      <c r="M30" t="str">
+      <c r="O30" t="str">
         <f t="shared" si="2"/>
         <v>daf-core-</v>
       </c>
-      <c r="N30" t="str">
+      <c r="P30" t="str">
         <f t="shared" si="6"/>
         <v>core-</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="I2:I16">
-    <sortCondition ref="I2:I16"/>
+  <sortState ref="K2:K16">
+    <sortCondition ref="K2:K16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2212,7 +2248,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>64</v>
@@ -2249,7 +2285,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -2654,7 +2690,7 @@
         <v>168</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>169</v>
@@ -2816,16 +2852,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" t="s">
         <v>171</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>172</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="13" t="s">
         <v>173</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>174</v>
       </c>
       <c r="G7" t="str">
         <f>"ValueSet/"&amp;C7&amp;".xml"</f>
@@ -3368,7 +3404,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
commit changes to birth sex binding.  build error
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9391 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FHIR_Build\guides\daf2\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885"/>
+    <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
@@ -23,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DAF-Research-Updates'!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
-  <calcPr calcId="171027" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="187">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -65,9 +60,6 @@
     <t>DiagnosticReport</t>
   </si>
   <si>
-    <t>Goals</t>
-  </si>
-  <si>
     <t>Immunization</t>
   </si>
   <si>
@@ -404,51 +396,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>daf-core-substance-ndfrt</t>
-  </si>
-  <si>
-    <t>daf-core-substance-rxnorm</t>
-  </si>
-  <si>
-    <t>daf-core-substance-sct</t>
-  </si>
-  <si>
-    <t>daf-core-substance-unii</t>
-  </si>
-  <si>
-    <t>daf-core-substance</t>
-  </si>
-  <si>
-    <t>DAF Core Substance ND-FRT codes</t>
-  </si>
-  <si>
-    <t>DAF Core Substance RxNorm Codes</t>
-  </si>
-  <si>
-    <t>DAF Core SNOMED CT Substances Other Than Clinical Drugs</t>
-  </si>
-  <si>
-    <t>DAF Core Substance UNII Codes</t>
-  </si>
-  <si>
-    <t>DAF Core Substance-Reactant for Intolerance and Negation Codes</t>
-  </si>
-  <si>
-    <t>substance-ndfrt</t>
-  </si>
-  <si>
-    <t>substance-rxnorm</t>
-  </si>
-  <si>
-    <t>substance-sct</t>
-  </si>
-  <si>
-    <t>substance-unii</t>
-  </si>
-  <si>
-    <t>substance</t>
-  </si>
-  <si>
     <t>id root</t>
   </si>
   <si>
@@ -533,27 +480,12 @@
     <t>Binding Name ( in spreadsheet)</t>
   </si>
   <si>
-    <t>DAFCoreAllergySubstance</t>
-  </si>
-  <si>
     <t>reference</t>
   </si>
   <si>
     <t>canonical-url</t>
   </si>
   <si>
-    <t>daf-race</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>Ethnicity group</t>
-  </si>
-  <si>
-    <t>DAFEthnicity</t>
-  </si>
-  <si>
     <t>spreadsheet reference</t>
   </si>
   <si>
@@ -627,13 +559,43 @@
   </si>
   <si>
     <t>Needs invariant</t>
+  </si>
+  <si>
+    <t>Birth Sex Extension</t>
+  </si>
+  <si>
+    <t>8/2/2016 needs wrapper</t>
+  </si>
+  <si>
+    <t>ONC required Birth Sex Codes</t>
+  </si>
+  <si>
+    <t>us-core-birth-sex</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>patient-daf-core-profile-spreadsheet.xml</t>
+  </si>
+  <si>
+    <t>birth-sex</t>
+  </si>
+  <si>
+    <t>Birth Sex Value Set</t>
+  </si>
+  <si>
+    <t>USBirthSex</t>
+  </si>
+  <si>
+    <t>daf-birth-sex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,6 +624,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -671,7 +639,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -688,11 +656,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -724,6 +707,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,14 +1011,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
@@ -1054,81 +1041,81 @@
     <col min="16" max="16" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
-        <v>69</v>
-      </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="F2" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>1</v>
@@ -1150,36 +1137,36 @@
         <v>core-allergyintolerance</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="I3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L3" t="s">
         <v>3</v>
@@ -1201,36 +1188,36 @@
         <v>core-careplan</v>
       </c>
       <c r="Q3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="H4" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L4" t="s">
         <v>2</v>
@@ -1252,36 +1239,36 @@
         <v>core-careteam</v>
       </c>
       <c r="Q4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="I5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
@@ -1292,36 +1279,36 @@
         <v>conformance-daf-core</v>
       </c>
       <c r="Q5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
         <v>74</v>
       </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="E6" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
@@ -1332,39 +1319,39 @@
         <v>documentreference-daf-core</v>
       </c>
       <c r="Q6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="H7" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="I7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J7" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="K7" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="L7" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
@@ -1375,39 +1362,39 @@
         <v>endpoint-daf-core</v>
       </c>
       <c r="Q7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="I8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J8" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="K8" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="L8" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
@@ -1426,36 +1413,36 @@
         <v>core-goal</v>
       </c>
       <c r="Q8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="H9" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
@@ -1474,36 +1461,36 @@
         <v>core-immunization</v>
       </c>
       <c r="Q9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="H10" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="I10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" t="s">
         <v>95</v>
       </c>
-      <c r="J10" t="s">
-        <v>96</v>
-      </c>
       <c r="K10" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="L10" t="s">
         <v>8</v>
@@ -1525,21 +1512,21 @@
         <v>core-device</v>
       </c>
       <c r="Q10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="1"/>
@@ -1550,10 +1537,10 @@
         <v>daf-</v>
       </c>
       <c r="Q11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1561,22 +1548,22 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E12" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="H12" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L12" t="s">
         <v>9</v>
@@ -1598,36 +1585,36 @@
         <v>core-diagnosticreport</v>
       </c>
       <c r="Q12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E13" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="J13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M13" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="1"/>
@@ -1642,36 +1629,36 @@
         <v>core-resultobs</v>
       </c>
       <c r="Q13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E14" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="H14" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="J14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
@@ -1690,21 +1677,21 @@
         <v>core-location</v>
       </c>
       <c r="Q14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="1"/>
@@ -1715,33 +1702,33 @@
         <v>daf-</v>
       </c>
       <c r="Q15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.75">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="J16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
@@ -1760,33 +1747,33 @@
         <v>core-medicationorder</v>
       </c>
       <c r="Q16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75">
       <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
@@ -1805,33 +1792,33 @@
         <v>core-medicationstatement</v>
       </c>
       <c r="Q17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="J18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
@@ -1850,36 +1837,36 @@
         <v>core-medication</v>
       </c>
       <c r="Q18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E19" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="H19" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="J19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
@@ -1898,36 +1885,36 @@
         <v>core-organization</v>
       </c>
       <c r="Q19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75">
       <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="H20" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
@@ -1946,36 +1933,36 @@
         <v>core-patient</v>
       </c>
       <c r="Q20" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="H21" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="J21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
@@ -1994,30 +1981,30 @@
         <v>core-pract</v>
       </c>
       <c r="Q21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.75">
       <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="J22" t="s">
         <v>7</v>
       </c>
       <c r="K22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L22" t="s">
         <v>7</v>
@@ -2039,36 +2026,36 @@
         <v>core-condition</v>
       </c>
       <c r="Q22" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="30">
       <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E23" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="J23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
@@ -2087,33 +2074,33 @@
         <v>core-procedure</v>
       </c>
       <c r="Q23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75">
       <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="J24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="0"/>
@@ -2132,36 +2119,36 @@
         <v>core-smokingstatus</v>
       </c>
       <c r="Q24" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="16.5" thickBot="1">
       <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E25" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="H25" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="0"/>
@@ -2180,21 +2167,65 @@
         <v>core-vitalsigns</v>
       </c>
       <c r="Q25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="16.5" thickBot="1">
+      <c r="A26" s="8">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>171</v>
+      </c>
+      <c r="H26" t="s">
+        <v>178</v>
+      </c>
+      <c r="J26" t="s">
+        <v>179</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="L26" t="s">
+        <v>181</v>
+      </c>
+      <c r="M26" t="s">
+        <v>182</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" ref="N26" si="6">K26&amp;"-daf-core"</f>
+        <v>us-core-birth-sex-daf-core</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" ref="O26" si="7">"daf-"&amp;P26</f>
+        <v>daf-core-us-core-birth-sex</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" ref="P26" si="8">"core-"&amp;K26</f>
+        <v>core-us-core-birth-sex</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75">
       <c r="B28" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="0"/>
@@ -2208,22 +2239,22 @@
         <v>daf-core-medicationdispense</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" ref="P28:P30" si="6">"core-"&amp;K28</f>
+        <f t="shared" ref="P28:P30" si="9">"core-"&amp;K28</f>
         <v>core-medicationdispense</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15.75">
       <c r="B29" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="0"/>
@@ -2237,19 +2268,19 @@
         <v>daf-core-medicationadministration</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>core-medicationadministration</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="B30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="0"/>
@@ -2263,7 +2294,7 @@
         <v>daf-core-</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>core-</v>
       </c>
     </row>
@@ -2277,14 +2308,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
@@ -2294,141 +2325,141 @@
     <col min="6" max="6" width="62.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>69</v>
       </c>
       <c r="D2" s="14">
         <v>42573</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
         <v>74</v>
       </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -2436,168 +2467,168 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75">
       <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="14">
         <v>42573</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
       <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75">
       <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75">
       <c r="B28" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75">
       <c r="B29" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="B30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2608,78 +2639,78 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2688,26 +2719,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
@@ -2718,404 +2749,160 @@
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>122</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>184</v>
+      </c>
+      <c r="F2" t="s">
+        <v>185</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G5" si="0">"ValueSet/"&amp;C2&amp;".xml"</f>
-        <v>ValueSet/daf-core-substance-ndfrt.xml</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ref="H2:H6" si="1">"valueset-"&amp;C2</f>
-        <v>valueset-daf-core-substance-ndfrt</v>
-      </c>
-      <c r="I2" t="str">
-        <f t="shared" ref="I2:I4" si="2">"http://hl7.org/fhir/daf/"&amp;G2</f>
-        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-ndfrt.xml</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>ValueSet/daf-core-substance-rxnorm.xml</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" si="1"/>
-        <v>valueset-daf-core-substance-rxnorm</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-rxnorm.xml</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>ValueSet/daf-core-substance-sct.xml</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" si="1"/>
-        <v>valueset-daf-core-substance-sct</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-sct.xml</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>ValueSet/daf-core-substance-unii.xml</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="1"/>
-        <v>valueset-daf-core-substance-unii</v>
-      </c>
-      <c r="I5" t="str">
-        <f>"http://hl7.org/fhir/daf/"&amp;G5</f>
-        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-unii.xml</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G6" t="str">
-        <f>"ValueSet/"&amp;C6&amp;".xml"</f>
-        <v>ValueSet/daf-core-substance.xml</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="1"/>
-        <v>valueset-daf-core-substance</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" ref="I6" si="3">"http://hl7.org/fhir/daf/"&amp;G6</f>
-        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance.xml</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="G7" t="str">
-        <f>"ValueSet/"&amp;C7&amp;".xml"</f>
-        <v>ValueSet/daf-race.xml</v>
-      </c>
-      <c r="H7" t="str">
-        <f>"valueset-"&amp;C7</f>
-        <v>valueset-daf-race</v>
-      </c>
-      <c r="I7" t="str">
-        <f>"http://hl7.org/fhir/daf/"&amp;G7</f>
-        <v>http://hl7.org/fhir/daf/ValueSet/daf-race.xml</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>10</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
+        <f>"valueset-daf-"&amp;D2</f>
+        <v>valueset-daf-birth-sex</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="8"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="8"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="8"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="8"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="8"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="8"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="8"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="8"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="8"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="8"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="8"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="8"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="8"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="8"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="8"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>14</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
-        <v>20</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>23</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3124,14 +2911,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
@@ -3141,49 +2928,49 @@
     <col min="8" max="9" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="b">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="str">
         <f>G3&amp;E3&amp;H3&amp;I3&amp;J3</f>
@@ -3196,28 +2983,28 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
         <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>57</v>
       </c>
       <c r="I3" t="str">
         <f>"daf-core-"&amp;F3</f>
         <v>daf-core-allergyintolerance</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="b">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C26" si="0">G4&amp;E4&amp;H4&amp;I4&amp;J4</f>
@@ -3230,28 +3017,28 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
         <v>56</v>
-      </c>
-      <c r="H4" t="s">
-        <v>57</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I26" si="1">"daf-core-"&amp;F4</f>
         <v>daf-core-careplan</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="b">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -3264,28 +3051,28 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
         <v>56</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-careteam</v>
+      </c>
+      <c r="J5" t="s">
         <v>57</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-careteam</v>
-      </c>
-      <c r="J5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="b">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -3298,62 +3085,62 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" t="s">
         <v>56</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-condition</v>
+      </c>
+      <c r="J6" t="s">
         <v>57</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-condition</v>
-      </c>
-      <c r="J6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="b">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>[Conformance](daf-core-conformance.html)</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" t="s">
         <v>56</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-conformance</v>
+      </c>
+      <c r="J7" t="s">
         <v>57</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-conformance</v>
-      </c>
-      <c r="J7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="b">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3363,31 +3150,31 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" t="s">
         <v>56</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-device</v>
+      </c>
+      <c r="J8" t="s">
         <v>57</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-device</v>
-      </c>
-      <c r="J8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="b">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3397,598 +3184,598 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
         <v>56</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-diagnosticreport</v>
+      </c>
+      <c r="J9" t="s">
         <v>57</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-diagnosticreport</v>
-      </c>
-      <c r="J9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="b">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>[DocumentReference](daf-core-documentreference.html)</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" t="s">
         <v>56</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-documentreference</v>
+      </c>
+      <c r="J10" t="s">
         <v>57</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-documentreference</v>
-      </c>
-      <c r="J10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="b">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>[Endpoint](daf-core-endpoint.html)</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E11" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F11" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" t="s">
         <v>56</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-endpoint</v>
+      </c>
+      <c r="J11" t="s">
         <v>57</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-endpoint</v>
-      </c>
-      <c r="J11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="b">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>[Goal](daf-core-goal.html)</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="F12" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
         <v>56</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-goal</v>
+      </c>
+      <c r="J12" t="s">
         <v>57</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-goal</v>
-      </c>
-      <c r="J12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="b">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>[Immunization](daf-core-immunization.html)</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" t="s">
         <v>56</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-immunization</v>
+      </c>
+      <c r="J13" t="s">
         <v>57</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-immunization</v>
-      </c>
-      <c r="J13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="b">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>[Location](daf-core-location.html)</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
         <v>56</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-location</v>
+      </c>
+      <c r="J14" t="s">
         <v>57</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-location</v>
-      </c>
-      <c r="J14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="b">
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>[](daf-core-.html)</v>
       </c>
       <c r="G15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" t="s">
         <v>56</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-</v>
+      </c>
+      <c r="J15" t="s">
         <v>57</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-</v>
-      </c>
-      <c r="J15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="b">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>[](daf-core-.html)</v>
       </c>
       <c r="G16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" t="s">
         <v>56</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-</v>
+      </c>
+      <c r="J16" t="s">
         <v>57</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-</v>
-      </c>
-      <c r="J16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="b">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>[Medication](daf-core-medication.html)</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" t="s">
         <v>56</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-medication</v>
+      </c>
+      <c r="J17" t="s">
         <v>57</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-medication</v>
-      </c>
-      <c r="J17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="b">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>[MedicationOrder](daf-core-medicationorder.html)</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
         <v>56</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-medicationorder</v>
+      </c>
+      <c r="J18" t="s">
         <v>57</v>
       </c>
-      <c r="I18" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-medicationorder</v>
-      </c>
-      <c r="J18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="b">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>[MedicationStatement](daf-core-medicationstatement.html)</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" t="s">
         <v>56</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-medicationstatement</v>
+      </c>
+      <c r="J19" t="s">
         <v>57</v>
       </c>
-      <c r="I19" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-medicationstatement</v>
-      </c>
-      <c r="J19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="b">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>[Observation-Results](daf-core-resultobs.html)</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" t="s">
         <v>56</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-resultobs</v>
+      </c>
+      <c r="J20" t="s">
         <v>57</v>
       </c>
-      <c r="I20" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-resultobs</v>
-      </c>
-      <c r="J20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="b">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>[Observation-Smokingstatus](daf-core-smokingstatus.html)</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" t="s">
         <v>56</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-smokingstatus</v>
+      </c>
+      <c r="J21" t="s">
         <v>57</v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-smokingstatus</v>
-      </c>
-      <c r="J21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="b">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>[Observation-Vitalsigns](daf-core-vitalsigns.html)</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" t="s">
         <v>56</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-vitalsigns</v>
+      </c>
+      <c r="J22" t="s">
         <v>57</v>
       </c>
-      <c r="I22" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-vitalsigns</v>
-      </c>
-      <c r="J22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="b">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>[Organization](daf-core-organization.html)</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" t="s">
         <v>56</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-organization</v>
+      </c>
+      <c r="J23" t="s">
         <v>57</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-organization</v>
-      </c>
-      <c r="J23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="b">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>[Patient](daf-core-patient.html)</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G24" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" t="s">
         <v>56</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-patient</v>
+      </c>
+      <c r="J24" t="s">
         <v>57</v>
       </c>
-      <c r="I24" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-patient</v>
-      </c>
-      <c r="J24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="b">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>[Practitioner](daf-core-pract.html)</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" t="s">
         <v>56</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-pract</v>
+      </c>
+      <c r="J25" t="s">
         <v>57</v>
       </c>
-      <c r="I25" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-pract</v>
-      </c>
-      <c r="J25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="b">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>[Procedure](daf-core-procedure.html)</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" t="s">
         <v>56</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v>daf-core-procedure</v>
+      </c>
+      <c r="J26" t="s">
         <v>57</v>
       </c>
-      <c r="I26" t="str">
-        <f t="shared" si="1"/>
-        <v>daf-core-procedure</v>
-      </c>
-      <c r="J26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10">
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5">
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5">
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>

</xml_diff>

<commit_message>
fix birth sex binding
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9394 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FHIR_Build\guides\daf2\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885" activeTab="4"/>
+    <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DAF-Research-Updates'!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
-  <calcPr calcId="125725" refMode="R1C1"/>
+  <calcPr calcId="171027" refMode="R1C1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="198">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -60,6 +65,9 @@
     <t>DiagnosticReport</t>
   </si>
   <si>
+    <t>Goals</t>
+  </si>
+  <si>
     <t>Immunization</t>
   </si>
   <si>
@@ -396,6 +404,51 @@
     <t>Title</t>
   </si>
   <si>
+    <t>daf-core-substance-ndfrt</t>
+  </si>
+  <si>
+    <t>daf-core-substance-rxnorm</t>
+  </si>
+  <si>
+    <t>daf-core-substance-sct</t>
+  </si>
+  <si>
+    <t>daf-core-substance-unii</t>
+  </si>
+  <si>
+    <t>daf-core-substance</t>
+  </si>
+  <si>
+    <t>DAF Core Substance ND-FRT codes</t>
+  </si>
+  <si>
+    <t>DAF Core Substance RxNorm Codes</t>
+  </si>
+  <si>
+    <t>DAF Core SNOMED CT Substances Other Than Clinical Drugs</t>
+  </si>
+  <si>
+    <t>DAF Core Substance UNII Codes</t>
+  </si>
+  <si>
+    <t>DAF Core Substance-Reactant for Intolerance and Negation Codes</t>
+  </si>
+  <si>
+    <t>substance-ndfrt</t>
+  </si>
+  <si>
+    <t>substance-rxnorm</t>
+  </si>
+  <si>
+    <t>substance-sct</t>
+  </si>
+  <si>
+    <t>substance-unii</t>
+  </si>
+  <si>
+    <t>substance</t>
+  </si>
+  <si>
     <t>id root</t>
   </si>
   <si>
@@ -480,12 +533,27 @@
     <t>Binding Name ( in spreadsheet)</t>
   </si>
   <si>
+    <t>DAFCoreAllergySubstance</t>
+  </si>
+  <si>
     <t>reference</t>
   </si>
   <si>
     <t>canonical-url</t>
   </si>
   <si>
+    <t>daf-race</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>Ethnicity group</t>
+  </si>
+  <si>
+    <t>DAFEthnicity</t>
+  </si>
+  <si>
     <t>spreadsheet reference</t>
   </si>
   <si>
@@ -559,43 +627,13 @@
   </si>
   <si>
     <t>Needs invariant</t>
-  </si>
-  <si>
-    <t>Birth Sex Extension</t>
-  </si>
-  <si>
-    <t>8/2/2016 needs wrapper</t>
-  </si>
-  <si>
-    <t>ONC required Birth Sex Codes</t>
-  </si>
-  <si>
-    <t>us-core-birth-sex</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>patient-daf-core-profile-spreadsheet.xml</t>
-  </si>
-  <si>
-    <t>birth-sex</t>
-  </si>
-  <si>
-    <t>Birth Sex Value Set</t>
-  </si>
-  <si>
-    <t>USBirthSex</t>
-  </si>
-  <si>
-    <t>daf-birth-sex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,12 +662,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -639,7 +671,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -656,26 +688,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -707,7 +724,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,17 +1027,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
@@ -1041,81 +1054,81 @@
     <col min="16" max="16" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>1</v>
@@ -1137,36 +1150,36 @@
         <v>core-allergyintolerance</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L3" t="s">
         <v>3</v>
@@ -1188,36 +1201,36 @@
         <v>core-careplan</v>
       </c>
       <c r="Q3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="H4" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="I4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L4" t="s">
         <v>2</v>
@@ -1239,36 +1252,36 @@
         <v>core-careteam</v>
       </c>
       <c r="Q4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
@@ -1279,36 +1292,36 @@
         <v>conformance-daf-core</v>
       </c>
       <c r="Q5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="E6" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="I6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
@@ -1319,39 +1332,39 @@
         <v>documentreference-daf-core</v>
       </c>
       <c r="Q6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
         <v>75</v>
       </c>
-      <c r="C7" t="s">
-        <v>74</v>
-      </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="H7" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="I7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J7" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="K7" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="L7" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
@@ -1362,39 +1375,39 @@
         <v>endpoint-daf-core</v>
       </c>
       <c r="Q7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="H8" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="I8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J8" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="K8" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="L8" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
@@ -1413,36 +1426,36 @@
         <v>core-goal</v>
       </c>
       <c r="Q8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="H9" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="J9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
@@ -1461,36 +1474,36 @@
         <v>core-immunization</v>
       </c>
       <c r="Q9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E10" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="H10" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="I10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K10" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="L10" t="s">
         <v>8</v>
@@ -1512,21 +1525,21 @@
         <v>core-device</v>
       </c>
       <c r="Q10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="1"/>
@@ -1537,10 +1550,10 @@
         <v>daf-</v>
       </c>
       <c r="Q11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1548,22 +1561,22 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="H12" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="J12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L12" t="s">
         <v>9</v>
@@ -1585,36 +1598,36 @@
         <v>core-diagnosticreport</v>
       </c>
       <c r="Q12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E13" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="J13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M13" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="1"/>
@@ -1629,36 +1642,36 @@
         <v>core-resultobs</v>
       </c>
       <c r="Q13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E14" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="H14" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="J14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
@@ -1677,21 +1690,21 @@
         <v>core-location</v>
       </c>
       <c r="Q14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="1"/>
@@ -1702,33 +1715,33 @@
         <v>daf-</v>
       </c>
       <c r="Q15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E16" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="J16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
@@ -1747,33 +1760,33 @@
         <v>core-medicationorder</v>
       </c>
       <c r="Q16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E17" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="J17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
@@ -1792,33 +1805,33 @@
         <v>core-medicationstatement</v>
       </c>
       <c r="Q17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E18" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="J18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
@@ -1837,36 +1850,36 @@
         <v>core-medication</v>
       </c>
       <c r="Q18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E19" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="H19" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
@@ -1885,36 +1898,36 @@
         <v>core-organization</v>
       </c>
       <c r="Q19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E20" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="H20" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="J20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="0"/>
@@ -1933,36 +1946,36 @@
         <v>core-patient</v>
       </c>
       <c r="Q20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E21" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="H21" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="J21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="0"/>
@@ -1981,30 +1994,30 @@
         <v>core-pract</v>
       </c>
       <c r="Q21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E22" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="J22" t="s">
         <v>7</v>
       </c>
       <c r="K22" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L22" t="s">
         <v>7</v>
@@ -2026,36 +2039,36 @@
         <v>core-condition</v>
       </c>
       <c r="Q22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="30">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E23" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="J23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="0"/>
@@ -2074,33 +2087,33 @@
         <v>core-procedure</v>
       </c>
       <c r="Q23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E24" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="J24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="0"/>
@@ -2119,36 +2132,36 @@
         <v>core-smokingstatus</v>
       </c>
       <c r="Q24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="16.5" thickBot="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E25" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="H25" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="J25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="0"/>
@@ -2167,65 +2180,21 @@
         <v>core-vitalsigns</v>
       </c>
       <c r="Q25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A26" s="8">
-        <v>24</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>171</v>
-      </c>
-      <c r="H26" t="s">
-        <v>178</v>
-      </c>
-      <c r="J26" t="s">
-        <v>179</v>
-      </c>
-      <c r="K26" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="L26" t="s">
-        <v>181</v>
-      </c>
-      <c r="M26" t="s">
-        <v>182</v>
-      </c>
-      <c r="N26" t="str">
-        <f t="shared" ref="N26" si="6">K26&amp;"-daf-core"</f>
-        <v>us-core-birth-sex-daf-core</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" ref="O26" si="7">"daf-"&amp;P26</f>
-        <v>daf-core-us-core-birth-sex</v>
-      </c>
-      <c r="P26" t="str">
-        <f t="shared" ref="P26" si="8">"core-"&amp;K26</f>
-        <v>core-us-core-birth-sex</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="15.75">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="0"/>
@@ -2239,22 +2208,22 @@
         <v>daf-core-medicationdispense</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" ref="P28:P30" si="9">"core-"&amp;K28</f>
+        <f t="shared" ref="P28:P30" si="6">"core-"&amp;K28</f>
         <v>core-medicationdispense</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75">
+    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="0"/>
@@ -2268,19 +2237,19 @@
         <v>daf-core-medicationadministration</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>core-medicationadministration</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="0"/>
@@ -2294,7 +2263,7 @@
         <v>daf-core-</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>core-</v>
       </c>
     </row>
@@ -2308,14 +2277,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
@@ -2325,141 +2294,141 @@
     <col min="6" max="6" width="62.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D2" s="14">
         <v>42573</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
         <v>75</v>
       </c>
-      <c r="C7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75">
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -2467,168 +2436,168 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" s="14">
         <v>42573</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75">
-      <c r="B29" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="B30" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2639,78 +2608,78 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2719,26 +2688,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
@@ -2749,160 +2718,404 @@
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>121</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G5" si="0">"ValueSet/"&amp;C2&amp;".xml"</f>
+        <v>ValueSet/daf-core-substance-ndfrt.xml</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H6" si="1">"valueset-"&amp;C2</f>
+        <v>valueset-daf-core-substance-ndfrt</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I4" si="2">"http://hl7.org/fhir/daf/"&amp;G2</f>
+        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-ndfrt.xml</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>ValueSet/daf-core-substance-rxnorm.xml</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="1"/>
+        <v>valueset-daf-core-substance-rxnorm</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-rxnorm.xml</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>ValueSet/daf-core-substance-sct.xml</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>valueset-daf-core-substance-sct</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
+        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-sct.xml</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>ValueSet/daf-core-substance-unii.xml</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>valueset-daf-core-substance-unii</v>
+      </c>
+      <c r="I5" t="str">
+        <f>"http://hl7.org/fhir/daf/"&amp;G5</f>
+        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-unii.xml</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" t="str">
+        <f>"ValueSet/"&amp;C6&amp;".xml"</f>
+        <v>ValueSet/daf-core-substance.xml</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>valueset-daf-core-substance</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ref="I6" si="3">"http://hl7.org/fhir/daf/"&amp;G6</f>
+        <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance.xml</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" t="str">
+        <f>"ValueSet/"&amp;C7&amp;".xml"</f>
+        <v>ValueSet/daf-race.xml</v>
+      </c>
+      <c r="H7" t="str">
+        <f>"valueset-"&amp;C7</f>
+        <v>valueset-daf-race</v>
+      </c>
+      <c r="I7" t="str">
+        <f>"http://hl7.org/fhir/daf/"&amp;G7</f>
+        <v>http://hl7.org/fhir/daf/ValueSet/daf-race.xml</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>10</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G2" t="str">
-        <f>"valueset-daf-"&amp;D2</f>
-        <v>valueset-daf-birth-sex</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="8"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="8"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="8"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="8"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="8"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="8"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="8"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="8"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="8"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="8"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="8"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="8"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="8"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="8"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="8"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="8"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="8"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="8"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="8"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="8"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="8"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="8"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="8"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="8"/>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2911,14 +3124,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
@@ -2928,49 +3141,49 @@
     <col min="8" max="9" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
       <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" t="str">
         <f>G3&amp;E3&amp;H3&amp;I3&amp;J3</f>
@@ -2983,28 +3196,28 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I3" t="str">
         <f>"daf-core-"&amp;F3</f>
         <v>daf-core-allergyintolerance</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C26" si="0">G4&amp;E4&amp;H4&amp;I4&amp;J4</f>
@@ -3017,28 +3230,28 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I26" si="1">"daf-core-"&amp;F4</f>
         <v>daf-core-careplan</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -3051,28 +3264,28 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-careteam</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -3085,62 +3298,62 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-condition</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>[Conformance](daf-core-conformance.html)</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-conformance</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3150,31 +3363,31 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-device</v>
       </c>
       <c r="J8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3184,598 +3397,598 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-diagnosticreport</v>
       </c>
       <c r="J9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>[DocumentReference](daf-core-documentreference.html)</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-documentreference</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>[Endpoint](daf-core-endpoint.html)</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="E11" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="F11" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-endpoint</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>[Goal](daf-core-goal.html)</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="F12" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-goal</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>[Immunization](daf-core-immunization.html)</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-immunization</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>[Location](daf-core-location.html)</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-location</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>[](daf-core-.html)</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>[](daf-core-.html)</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-</v>
       </c>
       <c r="J16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>[Medication](daf-core-medication.html)</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-medication</v>
       </c>
       <c r="J17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>[MedicationOrder](daf-core-medicationorder.html)</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-medicationorder</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>[MedicationStatement](daf-core-medicationstatement.html)</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-medicationstatement</v>
       </c>
       <c r="J19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>[Observation-Results](daf-core-resultobs.html)</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-resultobs</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>[Observation-Smokingstatus](daf-core-smokingstatus.html)</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-smokingstatus</v>
       </c>
       <c r="J21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>[Observation-Vitalsigns](daf-core-vitalsigns.html)</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-vitalsigns</v>
       </c>
       <c r="J22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>[Organization](daf-core-organization.html)</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-organization</v>
       </c>
       <c r="J23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>[Patient](daf-core-patient.html)</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-patient</v>
       </c>
       <c r="J24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>[Practitioner](daf-core-pract.html)</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-pract</v>
       </c>
       <c r="J25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>[Procedure](daf-core-procedure.html)</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
         <v>daf-core-procedure</v>
       </c>
       <c r="J26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="35" spans="4:5">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="4:5">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="38" spans="4:5">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>

</xml_diff>

<commit_message>
fix birth sex links
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9396 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FHIR_Build\guides\daf2\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885"/>
   </bookViews>
@@ -23,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DAF-Research-Updates'!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
-  <calcPr calcId="171027" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="203">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -578,9 +573,6 @@
     <t>bam: partial</t>
   </si>
   <si>
-    <t>7/21/2016 bam: Is race extension correct?</t>
-  </si>
-  <si>
     <t xml:space="preserve">7/21/2016 bam: Text Summary, and html guidance is broken. </t>
   </si>
   <si>
@@ -627,13 +619,31 @@
   </si>
   <si>
     <t>Needs invariant</t>
+  </si>
+  <si>
+    <t>DAF Core Birth Sex</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: Is race extension correct? 8/3/2016: EH  fixed binding and working on extension display</t>
+  </si>
+  <si>
+    <t>ONC required Birth Sex Codes</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>patient-daf-core-profile-spreadsheet.xml</t>
+  </si>
+  <si>
+    <t>birth-sex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +670,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -692,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -724,6 +740,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,14 +1044,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26:Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
@@ -1049,12 +1066,12 @@
     <col min="11" max="11" width="37.42578125" customWidth="1"/>
     <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="57" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -1068,7 +1085,7 @@
         <v>65</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>66</v>
@@ -1105,7 +1122,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1119,7 +1136,7 @@
         <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F2" t="s">
         <v>175</v>
@@ -1153,7 +1170,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1167,10 +1184,10 @@
         <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I3" t="s">
         <v>95</v>
@@ -1189,7 +1206,7 @@
         <v>careplan-daf-core-profile-spreadsheet.xml</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N25" si="1">K3&amp;"-daf-core"</f>
+        <f t="shared" ref="N3:N26" si="1">K3&amp;"-daf-core"</f>
         <v>careplan-daf-core</v>
       </c>
       <c r="O3" t="str">
@@ -1197,14 +1214,14 @@
         <v>daf-core-careplan</v>
       </c>
       <c r="P3" t="str">
-        <f t="shared" ref="P3:P25" si="3">"core-"&amp;K3</f>
+        <f t="shared" ref="P3:P26" si="3">"core-"&amp;K3</f>
         <v>core-careplan</v>
       </c>
       <c r="Q3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1218,7 +1235,7 @@
         <v>179</v>
       </c>
       <c r="E4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H4" t="s">
         <v>176</v>
@@ -1255,7 +1272,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.75">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1269,7 +1286,7 @@
         <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I5" t="s">
         <v>95</v>
@@ -1295,7 +1312,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.75">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1306,10 +1323,10 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I6" t="s">
         <v>95</v>
@@ -1335,7 +1352,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.75">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1346,10 +1363,10 @@
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H7" t="s">
         <v>144</v>
@@ -1378,7 +1395,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.75">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1392,7 +1409,7 @@
         <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H8" t="s">
         <v>178</v>
@@ -1429,7 +1446,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15.75">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1443,7 +1460,7 @@
         <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H9" t="s">
         <v>177</v>
@@ -1477,7 +1494,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15.75">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1491,7 +1508,7 @@
         <v>179</v>
       </c>
       <c r="E10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H10" t="s">
         <v>178</v>
@@ -1528,7 +1545,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15.75">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1553,7 +1570,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15.75">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1567,10 +1584,10 @@
         <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J12" t="s">
         <v>31</v>
@@ -1601,7 +1618,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15.75">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1615,7 +1632,7 @@
         <v>179</v>
       </c>
       <c r="E13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J13" t="s">
         <v>14</v>
@@ -1645,7 +1662,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15.75">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1659,10 +1676,10 @@
         <v>179</v>
       </c>
       <c r="E14" t="s">
+        <v>192</v>
+      </c>
+      <c r="H14" t="s">
         <v>193</v>
-      </c>
-      <c r="H14" t="s">
-        <v>194</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
@@ -1693,7 +1710,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15.75">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -1718,7 +1735,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15.75">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1732,7 +1749,7 @@
         <v>179</v>
       </c>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J16" t="s">
         <v>24</v>
@@ -1763,7 +1780,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="15.75">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1777,7 +1794,7 @@
         <v>179</v>
       </c>
       <c r="E17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
@@ -1808,7 +1825,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="15.75">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1822,7 +1839,7 @@
         <v>179</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J18" t="s">
         <v>13</v>
@@ -1853,7 +1870,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="15.75">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -1867,10 +1884,10 @@
         <v>179</v>
       </c>
       <c r="E19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19" t="s">
         <v>193</v>
-      </c>
-      <c r="H19" t="s">
-        <v>194</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
@@ -1901,7 +1918,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="15.75">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1915,10 +1932,10 @@
         <v>179</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H20" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="J20" t="s">
         <v>19</v>
@@ -1949,7 +1966,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="15.75">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -1963,10 +1980,10 @@
         <v>179</v>
       </c>
       <c r="E21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
@@ -1997,7 +2014,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="15.75">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -2011,7 +2028,7 @@
         <v>179</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J22" t="s">
         <v>7</v>
@@ -2042,7 +2059,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="30">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -2056,10 +2073,10 @@
         <v>179</v>
       </c>
       <c r="E23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J23" t="s">
         <v>21</v>
@@ -2090,7 +2107,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="15.75">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -2104,7 +2121,7 @@
         <v>179</v>
       </c>
       <c r="E24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J24" t="s">
         <v>16</v>
@@ -2135,7 +2152,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="15.75">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -2149,10 +2166,10 @@
         <v>179</v>
       </c>
       <c r="E25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J25" t="s">
         <v>17</v>
@@ -2172,18 +2189,59 @@
         <v>vitalsigns-daf-core</v>
       </c>
       <c r="O25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="O25:O26" si="6">"daf-"&amp;P25</f>
         <v>daf-core-vitalsigns</v>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="P25:P26" si="7">"core-"&amp;K25</f>
         <v>core-vitalsigns</v>
       </c>
       <c r="Q25" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="15.75">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" t="s">
+        <v>95</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="K26" t="s">
+        <v>202</v>
+      </c>
+      <c r="L26" t="s">
+        <v>200</v>
+      </c>
+      <c r="M26" t="s">
+        <v>201</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="1"/>
+        <v>birth-sex-daf-core</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="6"/>
+        <v>daf-core-birth-sex</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="7"/>
+        <v>core-birth-sex</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75">
       <c r="B28" s="6" t="s">
         <v>93</v>
       </c>
@@ -2208,11 +2266,11 @@
         <v>daf-core-medicationdispense</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" ref="P28:P30" si="6">"core-"&amp;K28</f>
+        <f t="shared" ref="P28:P30" si="8">"core-"&amp;K28</f>
         <v>core-medicationdispense</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15.75">
       <c r="B29" s="6" t="s">
         <v>93</v>
       </c>
@@ -2237,11 +2295,11 @@
         <v>daf-core-medicationadministration</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>core-medicationadministration</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="B30" t="s">
         <v>92</v>
       </c>
@@ -2263,7 +2321,7 @@
         <v>daf-core-</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>core-</v>
       </c>
     </row>
@@ -2277,14 +2335,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
@@ -2294,12 +2352,12 @@
     <col min="6" max="6" width="62.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>64</v>
@@ -2314,7 +2372,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2328,7 +2386,7 @@
         <v>42573</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -2336,11 +2394,11 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -2351,7 +2409,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -2362,7 +2420,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -2373,7 +2431,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -2384,7 +2442,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -2395,7 +2453,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -2406,7 +2464,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -2417,7 +2475,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -2428,7 +2486,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -2439,7 +2497,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -2450,7 +2508,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -2461,7 +2519,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -2472,7 +2530,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -2483,7 +2541,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -2494,7 +2552,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -2505,7 +2563,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.75">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -2516,7 +2574,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.75">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -2530,7 +2588,7 @@
         <v>42573</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -2541,7 +2599,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -2552,7 +2610,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.75">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -2563,7 +2621,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -2574,7 +2632,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15.75">
       <c r="A25" s="8">
         <v>24</v>
       </c>
@@ -2585,17 +2643,17 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.75">
       <c r="B28" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.75">
       <c r="B29" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="B30" t="s">
         <v>92</v>
       </c>
@@ -2608,20 +2666,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>147</v>
       </c>
@@ -2629,7 +2687,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -2637,7 +2695,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
         <v>146</v>
       </c>
@@ -2645,7 +2703,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="9" t="s">
         <v>149</v>
       </c>
@@ -2653,12 +2711,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -2666,7 +2724,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
         <v>157</v>
       </c>
@@ -2674,7 +2732,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
         <v>158</v>
       </c>
@@ -2688,26 +2746,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
@@ -2718,7 +2776,7 @@
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2747,7 +2805,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2776,7 +2834,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-ndfrt.xml</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2805,7 +2863,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-rxnorm.xml</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -2834,7 +2892,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-sct.xml</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2863,7 +2921,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance-unii.xml</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>1</v>
       </c>
@@ -2895,7 +2953,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-core-substance.xml</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -2927,7 +2985,7 @@
         <v>http://hl7.org/fhir/daf/ValueSet/daf-race.xml</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -2935,7 +2993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -2943,7 +3001,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="8">
         <v>5</v>
       </c>
@@ -2951,7 +3009,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="8">
         <v>6</v>
       </c>
@@ -2959,7 +3017,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="8">
         <v>7</v>
       </c>
@@ -2967,7 +3025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="8">
         <v>8</v>
       </c>
@@ -2975,7 +3033,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="8">
         <v>9</v>
       </c>
@@ -2983,7 +3041,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="8">
         <v>10</v>
       </c>
@@ -2991,7 +3049,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="8">
         <v>11</v>
       </c>
@@ -2999,7 +3057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="8">
         <v>12</v>
       </c>
@@ -3007,7 +3065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="8">
         <v>13</v>
       </c>
@@ -3015,7 +3073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="8">
         <v>14</v>
       </c>
@@ -3023,7 +3081,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="8">
         <v>15</v>
       </c>
@@ -3031,7 +3089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="8">
         <v>16</v>
       </c>
@@ -3039,7 +3097,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="8">
         <v>17</v>
       </c>
@@ -3047,7 +3105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="8">
         <v>18</v>
       </c>
@@ -3055,7 +3113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="8">
         <v>19</v>
       </c>
@@ -3063,7 +3121,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="8">
         <v>20</v>
       </c>
@@ -3071,7 +3129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="8">
         <v>21</v>
       </c>
@@ -3079,7 +3137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="8">
         <v>22</v>
       </c>
@@ -3087,7 +3145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="8">
         <v>23</v>
       </c>
@@ -3095,7 +3153,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="8">
         <v>24</v>
       </c>
@@ -3103,17 +3161,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="B32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2">
       <c r="B33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
         <v>15</v>
       </c>
@@ -3124,14 +3182,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
@@ -3141,7 +3199,7 @@
     <col min="8" max="9" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>163</v>
       </c>
@@ -3161,7 +3219,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -3178,7 +3236,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -3212,7 +3270,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -3246,7 +3304,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -3280,7 +3338,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -3314,7 +3372,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -3348,7 +3406,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -3382,7 +3440,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -3416,7 +3474,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -3450,7 +3508,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -3484,7 +3542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -3518,7 +3576,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -3552,7 +3610,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -3586,7 +3644,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -3611,7 +3669,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -3636,7 +3694,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -3670,7 +3728,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="b">
         <v>1</v>
       </c>
@@ -3704,7 +3762,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="b">
         <v>1</v>
       </c>
@@ -3738,7 +3796,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -3772,7 +3830,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" t="b">
         <v>1</v>
       </c>
@@ -3806,7 +3864,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -3840,7 +3898,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -3874,7 +3932,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -3908,7 +3966,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" t="b">
         <v>1</v>
       </c>
@@ -3942,7 +4000,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" t="b">
         <v>1</v>
       </c>
@@ -3976,19 +4034,19 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5">
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5">
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>

</xml_diff>

<commit_message>
updates links to examples and add patient example
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9399 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="205">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -637,6 +637,12 @@
   </si>
   <si>
     <t>birth-sex</t>
+  </si>
+  <si>
+    <t>na1</t>
+  </si>
+  <si>
+    <t>na2</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26:Q26"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1552,11 +1558,11 @@
       <c r="B11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>90</v>
+      <c r="J11" t="s">
+        <v>203</v>
+      </c>
+      <c r="L11" t="s">
+        <v>203</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="1"/>
@@ -1717,11 +1723,11 @@
       <c r="B15" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="J15" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>90</v>
+      <c r="J15" t="s">
+        <v>204</v>
+      </c>
+      <c r="L15" t="s">
+        <v>204</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="1"/>
@@ -2231,11 +2237,10 @@
       </c>
       <c r="O26" t="str">
         <f t="shared" si="6"/>
-        <v>daf-core-birth-sex</v>
-      </c>
-      <c r="P26" t="str">
-        <f t="shared" si="7"/>
-        <v>core-birth-sex</v>
+        <v>daf-birth-sex</v>
+      </c>
+      <c r="P26" t="s">
+        <v>202</v>
       </c>
       <c r="Q26" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
add code system for code extensions
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9403 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -573,9 +573,6 @@
     <t>bam: partial</t>
   </si>
   <si>
-    <t xml:space="preserve">7/21/2016 bam: Text Summary, and html guidance is broken. </t>
-  </si>
-  <si>
     <t>DAF Research Profiles</t>
   </si>
   <si>
@@ -643,6 +640,9 @@
   </si>
   <si>
     <t>na2</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: Text Summary, and html guidance is broken. 8/3/2016 EH: Category codes need work</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1091,7 +1091,7 @@
         <v>65</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>66</v>
@@ -1142,7 +1142,7 @@
         <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F2" t="s">
         <v>175</v>
@@ -1176,7 +1176,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75">
+    <row r="3" spans="1:17" ht="30">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1190,10 +1190,10 @@
         <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="I3" t="s">
         <v>95</v>
@@ -1241,7 +1241,7 @@
         <v>179</v>
       </c>
       <c r="E4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H4" t="s">
         <v>176</v>
@@ -1292,7 +1292,7 @@
         <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I5" t="s">
         <v>95</v>
@@ -1329,10 +1329,10 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I6" t="s">
         <v>95</v>
@@ -1369,10 +1369,10 @@
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H7" t="s">
         <v>144</v>
@@ -1415,7 +1415,7 @@
         <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H8" t="s">
         <v>178</v>
@@ -1466,7 +1466,7 @@
         <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H9" t="s">
         <v>177</v>
@@ -1514,7 +1514,7 @@
         <v>179</v>
       </c>
       <c r="E10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H10" t="s">
         <v>178</v>
@@ -1559,10 +1559,10 @@
         <v>80</v>
       </c>
       <c r="J11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="1"/>
@@ -1590,10 +1590,10 @@
         <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J12" t="s">
         <v>31</v>
@@ -1638,7 +1638,7 @@
         <v>179</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J13" t="s">
         <v>14</v>
@@ -1682,10 +1682,10 @@
         <v>179</v>
       </c>
       <c r="E14" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14" t="s">
         <v>192</v>
-      </c>
-      <c r="H14" t="s">
-        <v>193</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
@@ -1724,10 +1724,10 @@
         <v>82</v>
       </c>
       <c r="J15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="1"/>
@@ -1755,7 +1755,7 @@
         <v>179</v>
       </c>
       <c r="E16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J16" t="s">
         <v>24</v>
@@ -1800,7 +1800,7 @@
         <v>179</v>
       </c>
       <c r="E17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
@@ -1845,7 +1845,7 @@
         <v>179</v>
       </c>
       <c r="E18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J18" t="s">
         <v>13</v>
@@ -1890,10 +1890,10 @@
         <v>179</v>
       </c>
       <c r="E19" t="s">
+        <v>191</v>
+      </c>
+      <c r="H19" t="s">
         <v>192</v>
-      </c>
-      <c r="H19" t="s">
-        <v>193</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
@@ -1938,10 +1938,10 @@
         <v>179</v>
       </c>
       <c r="E20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J20" t="s">
         <v>19</v>
@@ -1986,10 +1986,10 @@
         <v>179</v>
       </c>
       <c r="E21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
@@ -2034,7 +2034,7 @@
         <v>179</v>
       </c>
       <c r="E22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J22" t="s">
         <v>7</v>
@@ -2079,10 +2079,10 @@
         <v>179</v>
       </c>
       <c r="E23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J23" t="s">
         <v>21</v>
@@ -2127,7 +2127,7 @@
         <v>179</v>
       </c>
       <c r="E24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J24" t="s">
         <v>16</v>
@@ -2172,10 +2172,10 @@
         <v>179</v>
       </c>
       <c r="E25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J25" t="s">
         <v>17</v>
@@ -2211,7 +2211,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C26" t="s">
         <v>71</v>
@@ -2220,16 +2220,16 @@
         <v>95</v>
       </c>
       <c r="J26" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="K26" t="s">
+        <v>201</v>
+      </c>
+      <c r="L26" t="s">
         <v>199</v>
       </c>
-      <c r="K26" t="s">
-        <v>202</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>200</v>
-      </c>
-      <c r="M26" t="s">
-        <v>201</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="1"/>
@@ -2240,7 +2240,7 @@
         <v>daf-birth-sex</v>
       </c>
       <c r="P26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q26" t="s">
         <v>140</v>
@@ -2362,7 +2362,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>64</v>
@@ -2399,7 +2399,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F3" s="2"/>
     </row>

</xml_diff>

<commit_message>
relax endpoint requirement, updated tracker
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@9568 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/guides/daf2/resources/daf-core-profiles.xlsx
+++ b/guides/daf2/resources/daf-core-profiles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="1680" windowWidth="25260" windowHeight="3885" activeTab="1"/>
+    <workbookView xWindow="-180" yWindow="1680" windowWidth="24180" windowHeight="3885"/>
   </bookViews>
   <sheets>
     <sheet name="Names-key" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DAF-Research-Updates'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Names-key'!$A$1:$Q$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Profiles-links'!$A$1:$J$26</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="208">
   <si>
     <t>spreadsheet filename</t>
   </si>
@@ -563,9 +564,6 @@
     <t>Quick review</t>
   </si>
   <si>
-    <t>7/21/2016 bam: Need value set for status, and roles</t>
-  </si>
-  <si>
     <t>7/21/2016 bam: Need value set for status, and VaccineCode</t>
   </si>
   <si>
@@ -647,10 +645,36 @@
     <t>na2</t>
   </si>
   <si>
-    <t>7/21/2016 bam: Text Summary, and html guidance is broken. 8/3/2016 EH: Category codes need work</t>
-  </si>
-  <si>
     <t>Dragon-I think we shold remove!</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: No additional value sets required. Html needs work
+8/8/2016 bam: already in order</t>
+  </si>
+  <si>
+    <t>8/8/2016 bam: - reordered elements and confirmed Argo requirements</t>
+  </si>
+  <si>
+    <t>7/21/2016 bam: Text Summary, and html guidance is broken. 
+8/3/2016 EH: Category codes need work
+8/8/2016 bam: - reordered elements and confirmed Argo requirements</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7/21/2016 bam: Need value set for status, and roles
+8/8/2016 bam: - reordered elements and confirmed Argo requirements. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name requirement on participant is a bit awkward.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -693,12 +717,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -722,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -755,6 +785,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1107,7 @@
     <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="62.42578125" customWidth="1"/>
+    <col min="8" max="8" width="70.42578125" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
     <col min="10" max="10" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37.42578125" customWidth="1"/>
@@ -1099,7 +1132,7 @@
         <v>65</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>66</v>
@@ -1147,13 +1180,16 @@
         <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F2" t="s">
         <v>175</v>
+      </c>
+      <c r="H2" t="s">
+        <v>205</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>1</v>
@@ -1184,7 +1220,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1195,13 +1231,13 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>204</v>
+        <v>189</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="I3" t="s">
         <v>95</v>
@@ -1235,7 +1271,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1246,13 +1282,13 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
-      </c>
-      <c r="H4" t="s">
-        <v>176</v>
+        <v>189</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="I4" t="s">
         <v>95</v>
@@ -1297,10 +1333,10 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I5" t="s">
         <v>95</v>
@@ -1337,10 +1373,10 @@
         <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I6" t="s">
         <v>95</v>
@@ -1377,10 +1413,10 @@
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H7" t="s">
         <v>144</v>
@@ -1409,7 +1445,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1420,13 +1456,13 @@
         <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
-        <v>191</v>
-      </c>
-      <c r="H8" t="s">
-        <v>178</v>
+        <v>190</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="I8" t="s">
         <v>95</v>
@@ -1471,13 +1507,13 @@
         <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -1519,13 +1555,13 @@
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I10" t="s">
         <v>95</v>
@@ -1567,10 +1603,10 @@
         <v>80</v>
       </c>
       <c r="J11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="1"/>
@@ -1595,13 +1631,13 @@
         <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J12" t="s">
         <v>31</v>
@@ -1643,10 +1679,10 @@
         <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J13" t="s">
         <v>14</v>
@@ -1687,13 +1723,13 @@
         <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H14" t="s">
         <v>191</v>
-      </c>
-      <c r="H14" t="s">
-        <v>192</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
@@ -1732,10 +1768,10 @@
         <v>82</v>
       </c>
       <c r="J15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="1"/>
@@ -1760,10 +1796,10 @@
         <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J16" t="s">
         <v>24</v>
@@ -1805,10 +1841,10 @@
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
@@ -1850,10 +1886,10 @@
         <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J18" t="s">
         <v>13</v>
@@ -1895,13 +1931,13 @@
         <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E19" t="s">
+        <v>190</v>
+      </c>
+      <c r="H19" t="s">
         <v>191</v>
-      </c>
-      <c r="H19" t="s">
-        <v>192</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
@@ -1943,13 +1979,13 @@
         <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J20" t="s">
         <v>19</v>
@@ -1991,13 +2027,13 @@
         <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
@@ -2039,10 +2075,10 @@
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J22" t="s">
         <v>7</v>
@@ -2084,13 +2120,13 @@
         <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J23" t="s">
         <v>21</v>
@@ -2132,10 +2168,10 @@
         <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J24" t="s">
         <v>16</v>
@@ -2177,13 +2213,13 @@
         <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J25" t="s">
         <v>17</v>
@@ -2219,7 +2255,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C26" t="s">
         <v>71</v>
@@ -2228,16 +2264,16 @@
         <v>95</v>
       </c>
       <c r="J26" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="K26" t="s">
+        <v>200</v>
+      </c>
+      <c r="L26" t="s">
         <v>198</v>
       </c>
-      <c r="K26" t="s">
-        <v>201</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>199</v>
-      </c>
-      <c r="M26" t="s">
-        <v>200</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="1"/>
@@ -2248,7 +2284,7 @@
         <v>daf-birth-sex</v>
       </c>
       <c r="P26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q26" t="s">
         <v>140</v>
@@ -2343,7 +2379,7 @@
     <sortCondition ref="K2:K16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2351,8 +2387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2370,7 +2406,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>64</v>
@@ -2407,7 +2443,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -2663,7 +2699,7 @@
         <v>69</v>
       </c>
       <c r="F24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2677,7 +2713,7 @@
         <v>69</v>
       </c>
       <c r="F25" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>